<commit_message>
added energy balance data for Indonesia energy profile display.
</commit_message>
<xml_diff>
--- a/data/raw/HEESI.xlsx
+++ b/data/raw/HEESI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Reference\code\DataViz\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D0F5853-BB92-40BB-B2DE-0EFCF9C93CD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CECC8E7-CE9E-478F-A75D-9343F9D29B8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HEESI ESDM" sheetId="33" r:id="rId1"/>
@@ -1915,6 +1915,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1939,35 +1943,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1996,6 +1979,30 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2011,14 +2018,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2029,6 +2036,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2038,27 +2054,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4955,10 +4955,10 @@
   <dimension ref="A1:V34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B22" sqref="B22"/>
+      <selection pane="bottomRight" activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7684,14 +7684,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="136" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="149" t="s">
+      <c r="A1" s="140" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="148" t="s">
         <v>325</v>
       </c>
-      <c r="C1" s="149"/>
-      <c r="D1" s="149"/>
+      <c r="C1" s="148"/>
+      <c r="D1" s="148"/>
       <c r="E1" t="s">
         <v>326</v>
       </c>
@@ -7700,7 +7700,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="136"/>
+      <c r="A2" s="140"/>
       <c r="B2" s="3" t="s">
         <v>323</v>
       </c>
@@ -10464,28 +10464,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:162" x14ac:dyDescent="0.25">
-      <c r="A1" s="166" t="s">
+      <c r="A1" s="173" t="s">
         <v>317</v>
       </c>
-      <c r="B1" s="166"/>
-      <c r="C1" s="166"/>
-      <c r="D1" s="166"/>
-      <c r="E1" s="166"/>
-      <c r="F1" s="166"/>
-      <c r="G1" s="166"/>
-      <c r="H1" s="166"/>
-      <c r="I1" s="166"/>
-      <c r="J1" s="166"/>
-      <c r="K1" s="166"/>
-      <c r="L1" s="166"/>
-      <c r="M1" s="166"/>
-      <c r="N1" s="166"/>
-      <c r="O1" s="166"/>
-      <c r="P1" s="166"/>
-      <c r="Q1" s="166"/>
-      <c r="R1" s="166"/>
-      <c r="S1" s="166"/>
-      <c r="T1" s="166"/>
+      <c r="B1" s="173"/>
+      <c r="C1" s="173"/>
+      <c r="D1" s="173"/>
+      <c r="E1" s="173"/>
+      <c r="F1" s="173"/>
+      <c r="G1" s="173"/>
+      <c r="H1" s="173"/>
+      <c r="I1" s="173"/>
+      <c r="J1" s="173"/>
+      <c r="K1" s="173"/>
+      <c r="L1" s="173"/>
+      <c r="M1" s="173"/>
+      <c r="N1" s="173"/>
+      <c r="O1" s="173"/>
+      <c r="P1" s="173"/>
+      <c r="Q1" s="173"/>
+      <c r="R1" s="173"/>
+      <c r="S1" s="173"/>
+      <c r="T1" s="173"/>
     </row>
     <row r="2" spans="1:162" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -11706,7 +11706,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="153" t="s">
+      <c r="A1" s="150" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="78" t="s">
@@ -11718,7 +11718,7 @@
       <c r="D1" s="78" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="144" t="s">
+      <c r="E1" s="162" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="79" t="s">
@@ -11732,18 +11732,18 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="153"/>
-      <c r="B2" s="169" t="s">
+      <c r="A2" s="150"/>
+      <c r="B2" s="174" t="s">
         <v>267</v>
       </c>
-      <c r="C2" s="169"/>
-      <c r="D2" s="169"/>
-      <c r="E2" s="144"/>
-      <c r="F2" s="170" t="s">
+      <c r="C2" s="174"/>
+      <c r="D2" s="174"/>
+      <c r="E2" s="162"/>
+      <c r="F2" s="175" t="s">
         <v>201</v>
       </c>
-      <c r="G2" s="170"/>
-      <c r="H2" s="170"/>
+      <c r="G2" s="175"/>
+      <c r="H2" s="175"/>
       <c r="I2">
         <v>1000000000</v>
       </c>
@@ -13383,27 +13383,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="139" t="s">
+      <c r="A1" s="143" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="139"/>
-      <c r="C1" s="139"/>
-      <c r="D1" s="139"/>
-      <c r="E1" s="134" t="s">
+      <c r="B1" s="143"/>
+      <c r="C1" s="143"/>
+      <c r="D1" s="143"/>
+      <c r="E1" s="138" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="138"/>
-      <c r="G1" s="135"/>
-      <c r="L1" s="141" t="s">
+      <c r="F1" s="142"/>
+      <c r="G1" s="139"/>
+      <c r="L1" s="145" t="s">
         <v>277</v>
       </c>
-      <c r="M1" s="141"/>
-      <c r="N1" s="141"/>
-      <c r="O1" s="141"/>
-      <c r="P1" s="141"/>
-      <c r="Q1" s="141"/>
-      <c r="R1" s="141"/>
-      <c r="S1" s="141"/>
+      <c r="M1" s="145"/>
+      <c r="N1" s="145"/>
+      <c r="O1" s="145"/>
+      <c r="P1" s="145"/>
+      <c r="Q1" s="145"/>
+      <c r="R1" s="145"/>
+      <c r="S1" s="145"/>
       <c r="AF1" s="67"/>
       <c r="AG1" s="55"/>
     </row>
@@ -15115,20 +15115,20 @@
       </c>
     </row>
     <row r="26" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A26" s="137" t="s">
+      <c r="A26" s="141" t="s">
         <v>59</v>
       </c>
-      <c r="B26" s="137"/>
-      <c r="C26" s="137"/>
-      <c r="D26" s="137"/>
-      <c r="E26" s="140" t="s">
+      <c r="B26" s="141"/>
+      <c r="C26" s="141"/>
+      <c r="D26" s="141"/>
+      <c r="E26" s="144" t="s">
         <v>236</v>
       </c>
-      <c r="F26" s="140"/>
-      <c r="G26" s="140" t="s">
+      <c r="F26" s="144"/>
+      <c r="G26" s="144" t="s">
         <v>235</v>
       </c>
-      <c r="H26" s="140"/>
+      <c r="H26" s="144"/>
       <c r="I26" s="85" t="s">
         <v>228</v>
       </c>
@@ -15178,14 +15178,14 @@
       <c r="H27" s="86" t="s">
         <v>233</v>
       </c>
-      <c r="I27" s="137" t="s">
+      <c r="I27" s="141" t="s">
         <v>14</v>
       </c>
-      <c r="J27" s="137"/>
-      <c r="K27" s="137"/>
-      <c r="L27" s="137"/>
-      <c r="M27" s="137"/>
-      <c r="N27" s="137"/>
+      <c r="J27" s="141"/>
+      <c r="K27" s="141"/>
+      <c r="L27" s="141"/>
+      <c r="M27" s="141"/>
+      <c r="N27" s="141"/>
       <c r="O27" s="85"/>
       <c r="P27" s="85"/>
       <c r="Q27" s="85"/>
@@ -16508,28 +16508,28 @@
       <c r="Q48" s="85"/>
     </row>
     <row r="50" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A50" s="136" t="s">
+      <c r="A50" s="140" t="s">
         <v>207</v>
       </c>
-      <c r="B50" s="136"/>
-      <c r="C50" s="136"/>
-      <c r="D50" s="136"/>
-      <c r="E50" s="136"/>
-      <c r="F50" s="136" t="s">
+      <c r="B50" s="140"/>
+      <c r="C50" s="140"/>
+      <c r="D50" s="140"/>
+      <c r="E50" s="140"/>
+      <c r="F50" s="140" t="s">
         <v>208</v>
       </c>
-      <c r="G50" s="136"/>
-      <c r="H50" s="136"/>
-      <c r="I50" s="136"/>
-      <c r="J50" s="136"/>
-      <c r="K50" s="136" t="s">
+      <c r="G50" s="140"/>
+      <c r="H50" s="140"/>
+      <c r="I50" s="140"/>
+      <c r="J50" s="140"/>
+      <c r="K50" s="140" t="s">
         <v>232</v>
       </c>
-      <c r="L50" s="136"/>
-      <c r="M50" s="136"/>
-      <c r="N50" s="136"/>
-      <c r="O50" s="136"/>
-      <c r="P50" s="136"/>
+      <c r="L50" s="140"/>
+      <c r="M50" s="140"/>
+      <c r="N50" s="140"/>
+      <c r="O50" s="140"/>
+      <c r="P50" s="140"/>
       <c r="Q50" s="72">
         <v>0.17960000000000001</v>
       </c>
@@ -17696,10 +17696,10 @@
       <c r="P72" s="3"/>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="G77" s="134" t="s">
+      <c r="G77" s="138" t="s">
         <v>382</v>
       </c>
-      <c r="H77" s="135"/>
+      <c r="H77" s="139"/>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
@@ -18417,33 +18417,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="171" t="s">
+      <c r="B1" s="176" t="s">
         <v>129</v>
       </c>
-      <c r="C1" s="171" t="s">
+      <c r="C1" s="176" t="s">
         <v>155</v>
       </c>
-      <c r="D1" s="171" t="s">
+      <c r="D1" s="176" t="s">
         <v>156</v>
       </c>
-      <c r="E1" s="171" t="s">
+      <c r="E1" s="176" t="s">
         <v>157</v>
       </c>
-      <c r="F1" s="171" t="s">
+      <c r="F1" s="176" t="s">
         <v>158</v>
       </c>
-      <c r="G1" s="171" t="s">
+      <c r="G1" s="176" t="s">
         <v>162</v>
       </c>
-      <c r="H1" s="171"/>
-      <c r="I1" s="171"/>
+      <c r="H1" s="176"/>
+      <c r="I1" s="176"/>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B2" s="171"/>
-      <c r="C2" s="171"/>
-      <c r="D2" s="171"/>
-      <c r="E2" s="171"/>
-      <c r="F2" s="171"/>
+      <c r="B2" s="176"/>
+      <c r="C2" s="176"/>
+      <c r="D2" s="176"/>
+      <c r="E2" s="176"/>
+      <c r="F2" s="176"/>
       <c r="G2" t="s">
         <v>159</v>
       </c>
@@ -19258,60 +19258,60 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="149" t="s">
+      <c r="A2" s="148" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="149"/>
-      <c r="C2" s="149"/>
-      <c r="D2" s="149"/>
-      <c r="E2" s="149"/>
-      <c r="F2" s="149"/>
-      <c r="G2" s="149"/>
-      <c r="H2" s="149"/>
-      <c r="I2" s="149"/>
-      <c r="J2" s="149"/>
-      <c r="K2" s="149"/>
-      <c r="L2" s="149"/>
+      <c r="B2" s="148"/>
+      <c r="C2" s="148"/>
+      <c r="D2" s="148"/>
+      <c r="E2" s="148"/>
+      <c r="F2" s="148"/>
+      <c r="G2" s="148"/>
+      <c r="H2" s="148"/>
+      <c r="I2" s="148"/>
+      <c r="J2" s="148"/>
+      <c r="K2" s="148"/>
+      <c r="L2" s="148"/>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="136" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="136" t="s">
+      <c r="A3" s="140" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="140" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="136" t="s">
+      <c r="C3" s="140" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="136" t="s">
+      <c r="D3" s="140" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="136" t="s">
+      <c r="E3" s="140" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="136" t="s">
+      <c r="F3" s="140" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="136"/>
-      <c r="H3" s="136"/>
-      <c r="I3" s="136"/>
-      <c r="J3" s="136"/>
-      <c r="K3" s="153" t="s">
+      <c r="G3" s="140"/>
+      <c r="H3" s="140"/>
+      <c r="I3" s="140"/>
+      <c r="J3" s="140"/>
+      <c r="K3" s="150" t="s">
         <v>90</v>
       </c>
-      <c r="L3" s="147" t="s">
+      <c r="L3" s="158" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="136" t="s">
+      <c r="M3" s="140" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="136"/>
-      <c r="B4" s="136"/>
-      <c r="C4" s="136"/>
-      <c r="D4" s="136"/>
-      <c r="E4" s="136"/>
+      <c r="A4" s="140"/>
+      <c r="B4" s="140"/>
+      <c r="C4" s="140"/>
+      <c r="D4" s="140"/>
+      <c r="E4" s="140"/>
       <c r="F4" s="2" t="s">
         <v>6</v>
       </c>
@@ -19327,28 +19327,28 @@
       <c r="J4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="153"/>
-      <c r="L4" s="148"/>
-      <c r="M4" s="136"/>
+      <c r="K4" s="150"/>
+      <c r="L4" s="159"/>
+      <c r="M4" s="140"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="136"/>
-      <c r="B5" s="149" t="s">
+      <c r="A5" s="140"/>
+      <c r="B5" s="148" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="149"/>
-      <c r="D5" s="149"/>
+      <c r="C5" s="148"/>
+      <c r="D5" s="148"/>
       <c r="E5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="172" t="s">
+      <c r="F5" s="180" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="173"/>
-      <c r="H5" s="173"/>
-      <c r="I5" s="173"/>
-      <c r="J5" s="173"/>
-      <c r="K5" s="174"/>
+      <c r="G5" s="181"/>
+      <c r="H5" s="181"/>
+      <c r="I5" s="181"/>
+      <c r="J5" s="181"/>
+      <c r="K5" s="182"/>
       <c r="L5" s="3" t="s">
         <v>16</v>
       </c>
@@ -20124,97 +20124,97 @@
       </c>
     </row>
     <row r="26" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A26" s="149" t="s">
+      <c r="A26" s="148" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="149"/>
-      <c r="C26" s="149"/>
-      <c r="D26" s="149"/>
-      <c r="E26" s="149"/>
-      <c r="F26" s="149"/>
-      <c r="G26" s="149"/>
-      <c r="H26" s="149"/>
-      <c r="I26" s="149"/>
-      <c r="J26" s="149"/>
-      <c r="K26" s="149"/>
-      <c r="L26" s="149"/>
+      <c r="B26" s="148"/>
+      <c r="C26" s="148"/>
+      <c r="D26" s="148"/>
+      <c r="E26" s="148"/>
+      <c r="F26" s="148"/>
+      <c r="G26" s="148"/>
+      <c r="H26" s="148"/>
+      <c r="I26" s="148"/>
+      <c r="J26" s="148"/>
+      <c r="K26" s="148"/>
+      <c r="L26" s="148"/>
       <c r="M26" s="3"/>
       <c r="AC26" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:38" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="136" t="s">
-        <v>0</v>
-      </c>
-      <c r="B27" s="136" t="s">
+      <c r="A27" s="140" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="140" t="s">
         <v>1</v>
       </c>
-      <c r="C27" s="136" t="s">
+      <c r="C27" s="140" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="136" t="s">
+      <c r="D27" s="140" t="s">
         <v>3</v>
       </c>
-      <c r="E27" s="136" t="s">
+      <c r="E27" s="140" t="s">
         <v>4</v>
       </c>
-      <c r="F27" s="136" t="s">
+      <c r="F27" s="140" t="s">
         <v>5</v>
       </c>
-      <c r="G27" s="136"/>
-      <c r="H27" s="136"/>
-      <c r="I27" s="136"/>
-      <c r="J27" s="136"/>
-      <c r="K27" s="150" t="s">
+      <c r="G27" s="140"/>
+      <c r="H27" s="140"/>
+      <c r="I27" s="140"/>
+      <c r="J27" s="140"/>
+      <c r="K27" s="146" t="s">
         <v>91</v>
       </c>
-      <c r="L27" s="147" t="s">
+      <c r="L27" s="158" t="s">
         <v>11</v>
       </c>
-      <c r="M27" s="147" t="s">
+      <c r="M27" s="158" t="s">
         <v>12</v>
       </c>
-      <c r="N27" s="147" t="s">
+      <c r="N27" s="158" t="s">
         <v>20</v>
       </c>
-      <c r="P27" s="153" t="s">
+      <c r="P27" s="150" t="s">
         <v>2</v>
       </c>
-      <c r="Q27" s="153" t="s">
+      <c r="Q27" s="150" t="s">
         <v>92</v>
       </c>
-      <c r="R27" s="153" t="s">
+      <c r="R27" s="150" t="s">
         <v>93</v>
       </c>
-      <c r="S27" s="153" t="s">
+      <c r="S27" s="150" t="s">
         <v>12</v>
       </c>
-      <c r="T27" s="153" t="s">
+      <c r="T27" s="150" t="s">
         <v>94</v>
       </c>
-      <c r="U27" s="136" t="s">
+      <c r="U27" s="140" t="s">
         <v>20</v>
       </c>
-      <c r="V27" s="144" t="s">
+      <c r="V27" s="162" t="s">
         <v>2</v>
       </c>
-      <c r="W27" s="144" t="s">
+      <c r="W27" s="162" t="s">
         <v>92</v>
       </c>
-      <c r="X27" s="144" t="s">
+      <c r="X27" s="162" t="s">
         <v>93</v>
       </c>
-      <c r="Y27" s="144" t="s">
+      <c r="Y27" s="162" t="s">
         <v>12</v>
       </c>
-      <c r="Z27" s="144" t="s">
+      <c r="Z27" s="162" t="s">
         <v>94</v>
       </c>
-      <c r="AA27" s="143" t="s">
+      <c r="AA27" s="161" t="s">
         <v>20</v>
       </c>
-      <c r="AC27" s="153" t="s">
+      <c r="AC27" s="150" t="s">
         <v>2</v>
       </c>
       <c r="AE27" s="20" t="s">
@@ -20234,11 +20234,11 @@
       </c>
     </row>
     <row r="28" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A28" s="136"/>
-      <c r="B28" s="136"/>
-      <c r="C28" s="136"/>
-      <c r="D28" s="136"/>
-      <c r="E28" s="136"/>
+      <c r="A28" s="140"/>
+      <c r="B28" s="140"/>
+      <c r="C28" s="140"/>
+      <c r="D28" s="140"/>
+      <c r="E28" s="140"/>
       <c r="F28" s="2" t="s">
         <v>6</v>
       </c>
@@ -20254,23 +20254,23 @@
       <c r="J28" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K28" s="151"/>
-      <c r="L28" s="148"/>
-      <c r="M28" s="148"/>
-      <c r="N28" s="148"/>
-      <c r="P28" s="153"/>
-      <c r="Q28" s="153"/>
-      <c r="R28" s="153"/>
-      <c r="S28" s="153"/>
-      <c r="T28" s="153"/>
-      <c r="U28" s="136"/>
-      <c r="V28" s="144"/>
-      <c r="W28" s="144"/>
-      <c r="X28" s="144"/>
-      <c r="Y28" s="144"/>
-      <c r="Z28" s="144"/>
-      <c r="AA28" s="143"/>
-      <c r="AC28" s="153"/>
+      <c r="K28" s="147"/>
+      <c r="L28" s="159"/>
+      <c r="M28" s="159"/>
+      <c r="N28" s="159"/>
+      <c r="P28" s="150"/>
+      <c r="Q28" s="150"/>
+      <c r="R28" s="150"/>
+      <c r="S28" s="150"/>
+      <c r="T28" s="150"/>
+      <c r="U28" s="140"/>
+      <c r="V28" s="162"/>
+      <c r="W28" s="162"/>
+      <c r="X28" s="162"/>
+      <c r="Y28" s="162"/>
+      <c r="Z28" s="162"/>
+      <c r="AA28" s="161"/>
+      <c r="AC28" s="150"/>
       <c r="AE28" s="20"/>
       <c r="AG28" s="20"/>
       <c r="AI28" s="20"/>
@@ -20278,38 +20278,38 @@
       <c r="AL28" s="2"/>
     </row>
     <row r="29" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A29" s="136"/>
-      <c r="B29" s="153" t="s">
+      <c r="A29" s="140"/>
+      <c r="B29" s="150" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="153"/>
-      <c r="D29" s="153"/>
-      <c r="E29" s="153"/>
-      <c r="F29" s="153"/>
-      <c r="G29" s="153"/>
-      <c r="H29" s="153"/>
-      <c r="I29" s="153"/>
-      <c r="J29" s="153"/>
-      <c r="K29" s="153"/>
-      <c r="L29" s="153"/>
-      <c r="M29" s="153"/>
-      <c r="N29" s="153"/>
-      <c r="P29" s="136" t="s">
+      <c r="C29" s="150"/>
+      <c r="D29" s="150"/>
+      <c r="E29" s="150"/>
+      <c r="F29" s="150"/>
+      <c r="G29" s="150"/>
+      <c r="H29" s="150"/>
+      <c r="I29" s="150"/>
+      <c r="J29" s="150"/>
+      <c r="K29" s="150"/>
+      <c r="L29" s="150"/>
+      <c r="M29" s="150"/>
+      <c r="N29" s="150"/>
+      <c r="P29" s="140" t="s">
         <v>19</v>
       </c>
-      <c r="Q29" s="136"/>
-      <c r="R29" s="136"/>
-      <c r="S29" s="136"/>
-      <c r="T29" s="136"/>
-      <c r="U29" s="136"/>
-      <c r="V29" s="143" t="s">
+      <c r="Q29" s="140"/>
+      <c r="R29" s="140"/>
+      <c r="S29" s="140"/>
+      <c r="T29" s="140"/>
+      <c r="U29" s="140"/>
+      <c r="V29" s="161" t="s">
         <v>95</v>
       </c>
-      <c r="W29" s="143"/>
-      <c r="X29" s="143"/>
-      <c r="Y29" s="143"/>
-      <c r="Z29" s="143"/>
-      <c r="AA29" s="143"/>
+      <c r="W29" s="161"/>
+      <c r="X29" s="161"/>
+      <c r="Y29" s="161"/>
+      <c r="Z29" s="161"/>
+      <c r="AA29" s="161"/>
     </row>
     <row r="30" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
@@ -22744,45 +22744,45 @@
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A51" s="149" t="s">
+      <c r="A51" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="B51" s="149"/>
-      <c r="C51" s="149"/>
-      <c r="D51" s="149"/>
-      <c r="E51" s="149"/>
-      <c r="F51" s="149"/>
-      <c r="G51" s="149"/>
-      <c r="H51" s="149"/>
-      <c r="I51" s="149"/>
-      <c r="J51" s="149"/>
-      <c r="K51" s="149"/>
-      <c r="L51" s="149"/>
-      <c r="M51" s="149"/>
+      <c r="B51" s="148"/>
+      <c r="C51" s="148"/>
+      <c r="D51" s="148"/>
+      <c r="E51" s="148"/>
+      <c r="F51" s="148"/>
+      <c r="G51" s="148"/>
+      <c r="H51" s="148"/>
+      <c r="I51" s="148"/>
+      <c r="J51" s="148"/>
+      <c r="K51" s="148"/>
+      <c r="L51" s="148"/>
+      <c r="M51" s="148"/>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A52" s="136" t="s">
-        <v>0</v>
-      </c>
-      <c r="B52" s="136" t="s">
+      <c r="A52" s="140" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" s="140" t="s">
         <v>2</v>
       </c>
-      <c r="C52" s="136" t="s">
+      <c r="C52" s="140" t="s">
         <v>3</v>
       </c>
-      <c r="D52" s="136" t="s">
+      <c r="D52" s="140" t="s">
         <v>4</v>
       </c>
-      <c r="E52" s="175" t="s">
+      <c r="E52" s="177" t="s">
         <v>5</v>
       </c>
-      <c r="F52" s="176"/>
-      <c r="G52" s="176"/>
-      <c r="H52" s="177"/>
-      <c r="I52" s="136" t="s">
+      <c r="F52" s="178"/>
+      <c r="G52" s="178"/>
+      <c r="H52" s="179"/>
+      <c r="I52" s="140" t="s">
         <v>11</v>
       </c>
-      <c r="J52" s="136" t="s">
+      <c r="J52" s="140" t="s">
         <v>12</v>
       </c>
       <c r="K52" s="3"/>
@@ -22790,10 +22790,10 @@
       <c r="M52" s="3"/>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A53" s="136"/>
-      <c r="B53" s="136"/>
-      <c r="C53" s="136"/>
-      <c r="D53" s="136"/>
+      <c r="A53" s="140"/>
+      <c r="B53" s="140"/>
+      <c r="C53" s="140"/>
+      <c r="D53" s="140"/>
       <c r="E53" s="2" t="s">
         <v>6</v>
       </c>
@@ -22806,8 +22806,8 @@
       <c r="H53" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I53" s="136"/>
-      <c r="J53" s="136"/>
+      <c r="I53" s="140"/>
+      <c r="J53" s="140"/>
       <c r="K53" s="3"/>
       <c r="L53" s="3"/>
       <c r="M53" s="3"/>
@@ -23166,23 +23166,21 @@
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="A2:L2"/>
-    <mergeCell ref="F3:J3"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="E52:H52"/>
-    <mergeCell ref="A51:M51"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="J52:J53"/>
-    <mergeCell ref="I52:I53"/>
-    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="AC27:AC28"/>
+    <mergeCell ref="X27:X28"/>
+    <mergeCell ref="Y27:Y28"/>
+    <mergeCell ref="Z27:Z28"/>
+    <mergeCell ref="AA27:AA28"/>
+    <mergeCell ref="V29:AA29"/>
+    <mergeCell ref="P29:U29"/>
+    <mergeCell ref="U27:U28"/>
+    <mergeCell ref="V27:V28"/>
+    <mergeCell ref="W27:W28"/>
+    <mergeCell ref="P27:P28"/>
+    <mergeCell ref="Q27:Q28"/>
+    <mergeCell ref="R27:R28"/>
+    <mergeCell ref="S27:S28"/>
+    <mergeCell ref="T27:T28"/>
     <mergeCell ref="M3:M4"/>
     <mergeCell ref="F5:K5"/>
     <mergeCell ref="M27:M28"/>
@@ -23198,21 +23196,23 @@
     <mergeCell ref="F27:J27"/>
     <mergeCell ref="K27:K28"/>
     <mergeCell ref="L27:L28"/>
-    <mergeCell ref="V29:AA29"/>
-    <mergeCell ref="P29:U29"/>
-    <mergeCell ref="U27:U28"/>
-    <mergeCell ref="V27:V28"/>
-    <mergeCell ref="W27:W28"/>
-    <mergeCell ref="P27:P28"/>
-    <mergeCell ref="Q27:Q28"/>
-    <mergeCell ref="R27:R28"/>
-    <mergeCell ref="S27:S28"/>
-    <mergeCell ref="T27:T28"/>
-    <mergeCell ref="AC27:AC28"/>
-    <mergeCell ref="X27:X28"/>
-    <mergeCell ref="Y27:Y28"/>
-    <mergeCell ref="Z27:Z28"/>
-    <mergeCell ref="AA27:AA28"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="E52:H52"/>
+    <mergeCell ref="A51:M51"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="J52:J53"/>
+    <mergeCell ref="I52:I53"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="F3:J3"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="A3:A5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -23245,15 +23245,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B2" s="149" t="s">
+      <c r="B2" s="148" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="149"/>
-      <c r="D2" s="149"/>
-      <c r="E2" s="149"/>
-      <c r="F2" s="149"/>
-      <c r="G2" s="149"/>
-      <c r="H2" s="149"/>
+      <c r="C2" s="148"/>
+      <c r="D2" s="148"/>
+      <c r="E2" s="148"/>
+      <c r="F2" s="148"/>
+      <c r="G2" s="148"/>
+      <c r="H2" s="148"/>
       <c r="N2" t="s">
         <v>102</v>
       </c>
@@ -23714,38 +23714,38 @@
       </c>
     </row>
     <row r="17" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="149" t="s">
+      <c r="B17" s="148" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="149"/>
-      <c r="D17" s="149"/>
-      <c r="E17" s="149"/>
-      <c r="F17" s="149"/>
-      <c r="G17" s="149"/>
-      <c r="H17" s="149"/>
-      <c r="I17" s="149"/>
+      <c r="C17" s="148"/>
+      <c r="D17" s="148"/>
+      <c r="E17" s="148"/>
+      <c r="F17" s="148"/>
+      <c r="G17" s="148"/>
+      <c r="H17" s="148"/>
+      <c r="I17" s="148"/>
       <c r="L17" t="s">
         <v>154</v>
       </c>
-      <c r="N17" s="153" t="s">
+      <c r="N17" s="150" t="s">
         <v>2</v>
       </c>
-      <c r="O17" s="153" t="s">
+      <c r="O17" s="150" t="s">
         <v>92</v>
       </c>
-      <c r="P17" s="153" t="s">
+      <c r="P17" s="150" t="s">
         <v>93</v>
       </c>
-      <c r="Q17" s="153" t="s">
+      <c r="Q17" s="150" t="s">
         <v>12</v>
       </c>
-      <c r="R17" s="153" t="s">
+      <c r="R17" s="150" t="s">
         <v>94</v>
       </c>
-      <c r="S17" s="136" t="s">
+      <c r="S17" s="140" t="s">
         <v>20</v>
       </c>
-      <c r="U17" s="153" t="s">
+      <c r="U17" s="150" t="s">
         <v>2</v>
       </c>
       <c r="W17" s="20" t="s">
@@ -23792,13 +23792,13 @@
       <c r="K18" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="N18" s="153"/>
-      <c r="O18" s="153"/>
-      <c r="P18" s="153"/>
-      <c r="Q18" s="153"/>
-      <c r="R18" s="153"/>
-      <c r="S18" s="136"/>
-      <c r="U18" s="153"/>
+      <c r="N18" s="150"/>
+      <c r="O18" s="150"/>
+      <c r="P18" s="150"/>
+      <c r="Q18" s="150"/>
+      <c r="R18" s="150"/>
+      <c r="S18" s="140"/>
+      <c r="U18" s="150"/>
       <c r="W18" s="20"/>
       <c r="Y18" s="20"/>
       <c r="AA18" s="20"/>
@@ -25507,14 +25507,14 @@
       </c>
     </row>
     <row r="39" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B39" s="149" t="s">
+      <c r="B39" s="148" t="s">
         <v>28</v>
       </c>
-      <c r="C39" s="149"/>
-      <c r="D39" s="149"/>
-      <c r="E39" s="149"/>
-      <c r="F39" s="149"/>
-      <c r="G39" s="149"/>
+      <c r="C39" s="148"/>
+      <c r="D39" s="148"/>
+      <c r="E39" s="148"/>
+      <c r="F39" s="148"/>
+      <c r="G39" s="148"/>
     </row>
     <row r="40" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B40" s="3" t="s">
@@ -25798,33 +25798,33 @@
       </c>
     </row>
     <row r="2" spans="2:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="141" t="s">
+      <c r="C2" s="145" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="141"/>
-      <c r="E2" s="141"/>
-      <c r="F2" s="141"/>
-      <c r="G2" s="141"/>
-      <c r="H2" s="141"/>
-      <c r="I2" s="141"/>
-      <c r="J2" s="141"/>
-      <c r="K2" s="141"/>
-      <c r="M2" s="153" t="s">
+      <c r="D2" s="145"/>
+      <c r="E2" s="145"/>
+      <c r="F2" s="145"/>
+      <c r="G2" s="145"/>
+      <c r="H2" s="145"/>
+      <c r="I2" s="145"/>
+      <c r="J2" s="145"/>
+      <c r="K2" s="145"/>
+      <c r="M2" s="150" t="s">
         <v>2</v>
       </c>
-      <c r="N2" s="153" t="s">
+      <c r="N2" s="150" t="s">
         <v>92</v>
       </c>
-      <c r="O2" s="153" t="s">
+      <c r="O2" s="150" t="s">
         <v>93</v>
       </c>
-      <c r="P2" s="153" t="s">
+      <c r="P2" s="150" t="s">
         <v>12</v>
       </c>
-      <c r="Q2" s="153" t="s">
+      <c r="Q2" s="150" t="s">
         <v>94</v>
       </c>
-      <c r="R2" s="136" t="s">
+      <c r="R2" s="140" t="s">
         <v>20</v>
       </c>
       <c r="T2" s="20" t="s">
@@ -25877,12 +25877,12 @@
       <c r="K3" t="s">
         <v>20</v>
       </c>
-      <c r="M3" s="153"/>
-      <c r="N3" s="153"/>
-      <c r="O3" s="153"/>
-      <c r="P3" s="153"/>
-      <c r="Q3" s="153"/>
-      <c r="R3" s="136"/>
+      <c r="M3" s="150"/>
+      <c r="N3" s="150"/>
+      <c r="O3" s="150"/>
+      <c r="P3" s="150"/>
+      <c r="Q3" s="150"/>
+      <c r="R3" s="140"/>
       <c r="T3" s="20"/>
       <c r="V3" s="20"/>
       <c r="X3" s="20"/>
@@ -27450,56 +27450,56 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C2" s="136" t="s">
+      <c r="C2" s="140" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="136"/>
-      <c r="E2" s="136"/>
-      <c r="F2" s="136"/>
-      <c r="G2" s="136"/>
-      <c r="H2" s="136"/>
-      <c r="I2" s="136"/>
-      <c r="J2" s="136"/>
-      <c r="K2" s="136"/>
-      <c r="L2" s="136"/>
-      <c r="M2" s="136"/>
-      <c r="N2" s="136"/>
-      <c r="O2" s="136"/>
-      <c r="P2" s="136"/>
-      <c r="Q2" s="136"/>
-      <c r="R2" s="136"/>
-      <c r="S2" s="136"/>
+      <c r="D2" s="140"/>
+      <c r="E2" s="140"/>
+      <c r="F2" s="140"/>
+      <c r="G2" s="140"/>
+      <c r="H2" s="140"/>
+      <c r="I2" s="140"/>
+      <c r="J2" s="140"/>
+      <c r="K2" s="140"/>
+      <c r="L2" s="140"/>
+      <c r="M2" s="140"/>
+      <c r="N2" s="140"/>
+      <c r="O2" s="140"/>
+      <c r="P2" s="140"/>
+      <c r="Q2" s="140"/>
+      <c r="R2" s="140"/>
+      <c r="S2" s="140"/>
     </row>
     <row r="3" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C3" s="136" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="136" t="s">
+      <c r="C3" s="140" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="140" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="136" t="s">
+      <c r="E3" s="140" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="136"/>
-      <c r="G3" s="136"/>
-      <c r="H3" s="136"/>
-      <c r="I3" s="136"/>
-      <c r="J3" s="136"/>
-      <c r="K3" s="136"/>
-      <c r="L3" s="136"/>
-      <c r="M3" s="136"/>
-      <c r="N3" s="136"/>
-      <c r="O3" s="136"/>
-      <c r="P3" s="136"/>
-      <c r="Q3" s="136"/>
-      <c r="R3" s="136"/>
-      <c r="S3" s="136" t="s">
+      <c r="F3" s="140"/>
+      <c r="G3" s="140"/>
+      <c r="H3" s="140"/>
+      <c r="I3" s="140"/>
+      <c r="J3" s="140"/>
+      <c r="K3" s="140"/>
+      <c r="L3" s="140"/>
+      <c r="M3" s="140"/>
+      <c r="N3" s="140"/>
+      <c r="O3" s="140"/>
+      <c r="P3" s="140"/>
+      <c r="Q3" s="140"/>
+      <c r="R3" s="140"/>
+      <c r="S3" s="140" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C4" s="136"/>
-      <c r="D4" s="136"/>
+      <c r="C4" s="140"/>
+      <c r="D4" s="140"/>
       <c r="E4" s="2" t="s">
         <v>30</v>
       </c>
@@ -27542,29 +27542,29 @@
       <c r="R4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="S4" s="136"/>
+      <c r="S4" s="140"/>
     </row>
     <row r="5" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C5" s="136"/>
+      <c r="C5" s="140"/>
       <c r="D5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="136" t="s">
+      <c r="E5" s="140" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="136"/>
-      <c r="G5" s="136"/>
-      <c r="H5" s="136"/>
-      <c r="I5" s="136"/>
-      <c r="J5" s="136"/>
-      <c r="K5" s="136"/>
-      <c r="L5" s="136"/>
-      <c r="M5" s="136"/>
-      <c r="N5" s="136"/>
-      <c r="O5" s="136"/>
-      <c r="P5" s="136"/>
-      <c r="Q5" s="136"/>
-      <c r="R5" s="136"/>
+      <c r="F5" s="140"/>
+      <c r="G5" s="140"/>
+      <c r="H5" s="140"/>
+      <c r="I5" s="140"/>
+      <c r="J5" s="140"/>
+      <c r="K5" s="140"/>
+      <c r="L5" s="140"/>
+      <c r="M5" s="140"/>
+      <c r="N5" s="140"/>
+      <c r="O5" s="140"/>
+      <c r="P5" s="140"/>
+      <c r="Q5" s="140"/>
+      <c r="R5" s="140"/>
       <c r="S5" s="2" t="s">
         <v>26</v>
       </c>
@@ -28153,42 +28153,42 @@
       </c>
     </row>
     <row r="18" spans="3:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="149" t="s">
+      <c r="C18" s="148" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="149"/>
-      <c r="E18" s="149"/>
-      <c r="F18" s="149"/>
-      <c r="G18" s="149"/>
-      <c r="H18" s="149"/>
-      <c r="I18" s="149"/>
-      <c r="J18" s="149"/>
-      <c r="K18" s="149"/>
-      <c r="L18" s="149"/>
-      <c r="M18" s="149"/>
-      <c r="N18" s="149"/>
-      <c r="O18" s="149"/>
-      <c r="P18" s="149"/>
-      <c r="Q18" s="149"/>
-      <c r="R18" s="149"/>
-      <c r="S18" s="149"/>
-      <c r="T18" s="149"/>
-      <c r="V18" s="153" t="s">
+      <c r="D18" s="148"/>
+      <c r="E18" s="148"/>
+      <c r="F18" s="148"/>
+      <c r="G18" s="148"/>
+      <c r="H18" s="148"/>
+      <c r="I18" s="148"/>
+      <c r="J18" s="148"/>
+      <c r="K18" s="148"/>
+      <c r="L18" s="148"/>
+      <c r="M18" s="148"/>
+      <c r="N18" s="148"/>
+      <c r="O18" s="148"/>
+      <c r="P18" s="148"/>
+      <c r="Q18" s="148"/>
+      <c r="R18" s="148"/>
+      <c r="S18" s="148"/>
+      <c r="T18" s="148"/>
+      <c r="V18" s="150" t="s">
         <v>2</v>
       </c>
-      <c r="W18" s="153" t="s">
+      <c r="W18" s="150" t="s">
         <v>92</v>
       </c>
-      <c r="X18" s="153" t="s">
+      <c r="X18" s="150" t="s">
         <v>93</v>
       </c>
-      <c r="Y18" s="153" t="s">
+      <c r="Y18" s="150" t="s">
         <v>12</v>
       </c>
-      <c r="Z18" s="153" t="s">
+      <c r="Z18" s="150" t="s">
         <v>94</v>
       </c>
-      <c r="AA18" s="136" t="s">
+      <c r="AA18" s="140" t="s">
         <v>20</v>
       </c>
       <c r="AC18" s="20" t="s">
@@ -28211,40 +28211,40 @@
       </c>
     </row>
     <row r="19" spans="3:38" x14ac:dyDescent="0.25">
-      <c r="C19" s="136" t="s">
-        <v>0</v>
-      </c>
-      <c r="D19" s="136" t="s">
+      <c r="C19" s="140" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="140" t="s">
         <v>4</v>
       </c>
-      <c r="E19" s="136" t="s">
+      <c r="E19" s="140" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="136"/>
-      <c r="G19" s="136"/>
-      <c r="H19" s="136"/>
-      <c r="I19" s="136"/>
-      <c r="J19" s="136"/>
-      <c r="K19" s="136"/>
-      <c r="L19" s="136"/>
-      <c r="M19" s="136"/>
-      <c r="N19" s="136"/>
-      <c r="O19" s="136"/>
-      <c r="P19" s="136"/>
-      <c r="Q19" s="136"/>
-      <c r="R19" s="136"/>
-      <c r="S19" s="136" t="s">
+      <c r="F19" s="140"/>
+      <c r="G19" s="140"/>
+      <c r="H19" s="140"/>
+      <c r="I19" s="140"/>
+      <c r="J19" s="140"/>
+      <c r="K19" s="140"/>
+      <c r="L19" s="140"/>
+      <c r="M19" s="140"/>
+      <c r="N19" s="140"/>
+      <c r="O19" s="140"/>
+      <c r="P19" s="140"/>
+      <c r="Q19" s="140"/>
+      <c r="R19" s="140"/>
+      <c r="S19" s="140" t="s">
         <v>12</v>
       </c>
-      <c r="T19" s="136" t="s">
+      <c r="T19" s="140" t="s">
         <v>20</v>
       </c>
-      <c r="V19" s="153"/>
-      <c r="W19" s="153"/>
-      <c r="X19" s="153"/>
-      <c r="Y19" s="153"/>
-      <c r="Z19" s="153"/>
-      <c r="AA19" s="136"/>
+      <c r="V19" s="150"/>
+      <c r="W19" s="150"/>
+      <c r="X19" s="150"/>
+      <c r="Y19" s="150"/>
+      <c r="Z19" s="150"/>
+      <c r="AA19" s="140"/>
       <c r="AC19" s="20"/>
       <c r="AE19" s="20"/>
       <c r="AG19" s="20"/>
@@ -28253,8 +28253,8 @@
       <c r="AL19" s="2"/>
     </row>
     <row r="20" spans="3:38" x14ac:dyDescent="0.25">
-      <c r="C20" s="136"/>
-      <c r="D20" s="136"/>
+      <c r="C20" s="140"/>
+      <c r="D20" s="140"/>
       <c r="E20" s="2" t="s">
         <v>30</v>
       </c>
@@ -28297,16 +28297,16 @@
       <c r="R20" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="S20" s="136"/>
-      <c r="T20" s="136"/>
-      <c r="V20" s="136" t="s">
+      <c r="S20" s="140"/>
+      <c r="T20" s="140"/>
+      <c r="V20" s="140" t="s">
         <v>95</v>
       </c>
-      <c r="W20" s="136"/>
-      <c r="X20" s="136"/>
-      <c r="Y20" s="136"/>
-      <c r="Z20" s="136"/>
-      <c r="AA20" s="136"/>
+      <c r="W20" s="140"/>
+      <c r="X20" s="140"/>
+      <c r="Y20" s="140"/>
+      <c r="Z20" s="140"/>
+      <c r="AA20" s="140"/>
       <c r="AC20" s="2" t="s">
         <v>101</v>
       </c>
@@ -30365,26 +30365,26 @@
       </c>
     </row>
     <row r="41" spans="3:42" x14ac:dyDescent="0.25">
-      <c r="C41" s="149" t="s">
+      <c r="C41" s="148" t="s">
         <v>42</v>
       </c>
-      <c r="D41" s="149"/>
-      <c r="E41" s="149"/>
-      <c r="F41" s="149"/>
-      <c r="G41" s="149"/>
-      <c r="H41" s="149"/>
-      <c r="I41" s="149"/>
-      <c r="J41" s="149"/>
-      <c r="K41" s="149"/>
-      <c r="L41" s="149"/>
-      <c r="M41" s="149"/>
-      <c r="N41" s="149"/>
-      <c r="O41" s="149"/>
-      <c r="P41" s="149"/>
-      <c r="Q41" s="149"/>
-      <c r="R41" s="149"/>
-      <c r="S41" s="149"/>
-      <c r="T41" s="149"/>
+      <c r="D41" s="148"/>
+      <c r="E41" s="148"/>
+      <c r="F41" s="148"/>
+      <c r="G41" s="148"/>
+      <c r="H41" s="148"/>
+      <c r="I41" s="148"/>
+      <c r="J41" s="148"/>
+      <c r="K41" s="148"/>
+      <c r="L41" s="148"/>
+      <c r="M41" s="148"/>
+      <c r="N41" s="148"/>
+      <c r="O41" s="148"/>
+      <c r="P41" s="148"/>
+      <c r="Q41" s="148"/>
+      <c r="R41" s="148"/>
+      <c r="S41" s="148"/>
+      <c r="T41" s="148"/>
       <c r="W41" t="s">
         <v>102</v>
       </c>
@@ -30447,32 +30447,32 @@
       </c>
     </row>
     <row r="42" spans="3:42" x14ac:dyDescent="0.25">
-      <c r="C42" s="136" t="s">
-        <v>0</v>
-      </c>
-      <c r="D42" s="136" t="s">
+      <c r="C42" s="140" t="s">
+        <v>0</v>
+      </c>
+      <c r="D42" s="140" t="s">
         <v>4</v>
       </c>
-      <c r="E42" s="136" t="s">
+      <c r="E42" s="140" t="s">
         <v>5</v>
       </c>
-      <c r="F42" s="136"/>
-      <c r="G42" s="136"/>
-      <c r="H42" s="136"/>
-      <c r="I42" s="136"/>
-      <c r="J42" s="136"/>
-      <c r="K42" s="136"/>
-      <c r="L42" s="136"/>
-      <c r="M42" s="136"/>
-      <c r="N42" s="136"/>
-      <c r="O42" s="136"/>
-      <c r="P42" s="136"/>
-      <c r="Q42" s="136"/>
-      <c r="R42" s="136"/>
-      <c r="S42" s="136" t="s">
+      <c r="F42" s="140"/>
+      <c r="G42" s="140"/>
+      <c r="H42" s="140"/>
+      <c r="I42" s="140"/>
+      <c r="J42" s="140"/>
+      <c r="K42" s="140"/>
+      <c r="L42" s="140"/>
+      <c r="M42" s="140"/>
+      <c r="N42" s="140"/>
+      <c r="O42" s="140"/>
+      <c r="P42" s="140"/>
+      <c r="Q42" s="140"/>
+      <c r="R42" s="140"/>
+      <c r="S42" s="140" t="s">
         <v>12</v>
       </c>
-      <c r="T42" s="136" t="s">
+      <c r="T42" s="140" t="s">
         <v>20</v>
       </c>
       <c r="W42" t="s">
@@ -30537,8 +30537,8 @@
       </c>
     </row>
     <row r="43" spans="3:42" x14ac:dyDescent="0.25">
-      <c r="C43" s="136"/>
-      <c r="D43" s="136"/>
+      <c r="C43" s="140"/>
+      <c r="D43" s="140"/>
       <c r="E43" s="2" t="s">
         <v>30</v>
       </c>
@@ -30581,8 +30581,8 @@
       <c r="R43" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="S43" s="136"/>
-      <c r="T43" s="136"/>
+      <c r="S43" s="140"/>
+      <c r="T43" s="140"/>
       <c r="W43" t="s">
         <v>104</v>
       </c>
@@ -31289,6 +31289,24 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="AA18:AA19"/>
+    <mergeCell ref="V20:AA20"/>
+    <mergeCell ref="V18:V19"/>
+    <mergeCell ref="W18:W19"/>
+    <mergeCell ref="X18:X19"/>
+    <mergeCell ref="Y18:Y19"/>
+    <mergeCell ref="Z18:Z19"/>
+    <mergeCell ref="C41:T41"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="E42:R42"/>
+    <mergeCell ref="S42:S43"/>
+    <mergeCell ref="T42:T43"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:R19"/>
+    <mergeCell ref="S19:S20"/>
+    <mergeCell ref="T19:T20"/>
+    <mergeCell ref="C19:C20"/>
     <mergeCell ref="C2:S2"/>
     <mergeCell ref="C18:T18"/>
     <mergeCell ref="S3:S4"/>
@@ -31296,24 +31314,6 @@
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:R3"/>
     <mergeCell ref="E5:R5"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:R19"/>
-    <mergeCell ref="S19:S20"/>
-    <mergeCell ref="T19:T20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="C41:T41"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="E42:R42"/>
-    <mergeCell ref="S42:S43"/>
-    <mergeCell ref="T42:T43"/>
-    <mergeCell ref="AA18:AA19"/>
-    <mergeCell ref="V20:AA20"/>
-    <mergeCell ref="V18:V19"/>
-    <mergeCell ref="W18:W19"/>
-    <mergeCell ref="X18:X19"/>
-    <mergeCell ref="Y18:Y19"/>
-    <mergeCell ref="Z18:Z19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -31335,65 +31335,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="J1" s="153" t="s">
+      <c r="J1" s="150" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="153" t="s">
+      <c r="K1" s="150" t="s">
         <v>92</v>
       </c>
-      <c r="L1" s="153" t="s">
+      <c r="L1" s="150" t="s">
         <v>93</v>
       </c>
-      <c r="M1" s="153" t="s">
+      <c r="M1" s="150" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="153" t="s">
+      <c r="N1" s="150" t="s">
         <v>94</v>
       </c>
-      <c r="O1" s="136" t="s">
+      <c r="O1" s="140" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="153" t="s">
+      <c r="Q1" s="150" t="s">
         <v>2</v>
       </c>
-      <c r="R1" s="153" t="s">
+      <c r="R1" s="150" t="s">
         <v>92</v>
       </c>
-      <c r="S1" s="153" t="s">
+      <c r="S1" s="150" t="s">
         <v>93</v>
       </c>
-      <c r="T1" s="153" t="s">
+      <c r="T1" s="150" t="s">
         <v>12</v>
       </c>
-      <c r="U1" s="153" t="s">
+      <c r="U1" s="150" t="s">
         <v>94</v>
       </c>
-      <c r="V1" s="136" t="s">
+      <c r="V1" s="140" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B2" s="173" t="s">
+      <c r="B2" s="181" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="173"/>
-      <c r="D2" s="173"/>
-      <c r="E2" s="173"/>
-      <c r="F2" s="173"/>
-      <c r="G2" s="173"/>
-      <c r="H2" s="173"/>
-      <c r="J2" s="153"/>
-      <c r="K2" s="153"/>
-      <c r="L2" s="153"/>
-      <c r="M2" s="153"/>
-      <c r="N2" s="153"/>
-      <c r="O2" s="136"/>
-      <c r="Q2" s="153"/>
-      <c r="R2" s="153"/>
-      <c r="S2" s="153"/>
-      <c r="T2" s="153"/>
-      <c r="U2" s="153"/>
-      <c r="V2" s="136"/>
+      <c r="C2" s="181"/>
+      <c r="D2" s="181"/>
+      <c r="E2" s="181"/>
+      <c r="F2" s="181"/>
+      <c r="G2" s="181"/>
+      <c r="H2" s="181"/>
+      <c r="J2" s="150"/>
+      <c r="K2" s="150"/>
+      <c r="L2" s="150"/>
+      <c r="M2" s="150"/>
+      <c r="N2" s="150"/>
+      <c r="O2" s="140"/>
+      <c r="Q2" s="150"/>
+      <c r="R2" s="150"/>
+      <c r="S2" s="150"/>
+      <c r="T2" s="150"/>
+      <c r="U2" s="150"/>
+      <c r="V2" s="140"/>
     </row>
     <row r="3" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
@@ -31417,22 +31417,22 @@
       <c r="H3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J3" s="136" t="s">
+      <c r="J3" s="140" t="s">
         <v>95</v>
       </c>
-      <c r="K3" s="136"/>
-      <c r="L3" s="136"/>
-      <c r="M3" s="136"/>
-      <c r="N3" s="136"/>
-      <c r="O3" s="136"/>
-      <c r="Q3" s="136" t="s">
+      <c r="K3" s="140"/>
+      <c r="L3" s="140"/>
+      <c r="M3" s="140"/>
+      <c r="N3" s="140"/>
+      <c r="O3" s="140"/>
+      <c r="Q3" s="140" t="s">
         <v>101</v>
       </c>
-      <c r="R3" s="136"/>
-      <c r="S3" s="136"/>
-      <c r="T3" s="136"/>
-      <c r="U3" s="136"/>
-      <c r="V3" s="136"/>
+      <c r="R3" s="140"/>
+      <c r="S3" s="140"/>
+      <c r="T3" s="140"/>
+      <c r="U3" s="140"/>
+      <c r="V3" s="140"/>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B4" s="3">
@@ -32568,102 +32568,102 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:23" x14ac:dyDescent="0.25">
-      <c r="C2" s="149" t="s">
+      <c r="C2" s="148" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="149"/>
-      <c r="E2" s="149"/>
-      <c r="F2" s="149"/>
-      <c r="G2" s="149"/>
-      <c r="H2" s="149"/>
-      <c r="I2" s="149"/>
-      <c r="J2" s="149"/>
-      <c r="K2" s="149"/>
-      <c r="L2" s="149"/>
-      <c r="M2" s="149"/>
-      <c r="N2" s="149"/>
-      <c r="O2" s="149"/>
-      <c r="P2" s="149"/>
-      <c r="Q2" s="149"/>
-      <c r="R2" s="149"/>
-      <c r="S2" s="149"/>
-      <c r="T2" s="149"/>
-      <c r="U2" s="149"/>
-      <c r="V2" s="149"/>
-      <c r="W2" s="149"/>
+      <c r="D2" s="148"/>
+      <c r="E2" s="148"/>
+      <c r="F2" s="148"/>
+      <c r="G2" s="148"/>
+      <c r="H2" s="148"/>
+      <c r="I2" s="148"/>
+      <c r="J2" s="148"/>
+      <c r="K2" s="148"/>
+      <c r="L2" s="148"/>
+      <c r="M2" s="148"/>
+      <c r="N2" s="148"/>
+      <c r="O2" s="148"/>
+      <c r="P2" s="148"/>
+      <c r="Q2" s="148"/>
+      <c r="R2" s="148"/>
+      <c r="S2" s="148"/>
+      <c r="T2" s="148"/>
+      <c r="U2" s="148"/>
+      <c r="V2" s="148"/>
+      <c r="W2" s="148"/>
     </row>
     <row r="3" spans="3:23" x14ac:dyDescent="0.25">
-      <c r="C3" s="136" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="136" t="s">
+      <c r="C3" s="140" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="140" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="136" t="s">
+      <c r="E3" s="140" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="136" t="s">
+      <c r="F3" s="140" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="136" t="s">
+      <c r="G3" s="140" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="136" t="s">
+      <c r="H3" s="140" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="136" t="s">
+      <c r="I3" s="140" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="136" t="s">
+      <c r="J3" s="140" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="136" t="s">
+      <c r="K3" s="140" t="s">
         <v>34</v>
       </c>
-      <c r="L3" s="136" t="s">
+      <c r="L3" s="140" t="s">
         <v>33</v>
       </c>
-      <c r="M3" s="136" t="s">
+      <c r="M3" s="140" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="136" t="s">
+      <c r="N3" s="140" t="s">
         <v>29</v>
       </c>
-      <c r="O3" s="136" t="s">
+      <c r="O3" s="140" t="s">
         <v>46</v>
       </c>
-      <c r="P3" s="136"/>
-      <c r="Q3" s="136"/>
-      <c r="R3" s="136"/>
-      <c r="S3" s="136" t="s">
+      <c r="P3" s="140"/>
+      <c r="Q3" s="140"/>
+      <c r="R3" s="140"/>
+      <c r="S3" s="140" t="s">
         <v>50</v>
       </c>
-      <c r="T3" s="136" t="s">
+      <c r="T3" s="140" t="s">
         <v>51</v>
       </c>
-      <c r="U3" s="136" t="s">
+      <c r="U3" s="140" t="s">
         <v>11</v>
       </c>
-      <c r="V3" s="136" t="s">
+      <c r="V3" s="140" t="s">
         <v>52</v>
       </c>
-      <c r="W3" s="153" t="s">
+      <c r="W3" s="150" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="4" spans="3:23" x14ac:dyDescent="0.25">
-      <c r="C4" s="136"/>
-      <c r="D4" s="136"/>
-      <c r="E4" s="136"/>
-      <c r="F4" s="136"/>
-      <c r="G4" s="136"/>
-      <c r="H4" s="136"/>
-      <c r="I4" s="136"/>
-      <c r="J4" s="136"/>
-      <c r="K4" s="136"/>
-      <c r="L4" s="136"/>
-      <c r="M4" s="136"/>
-      <c r="N4" s="136"/>
+      <c r="C4" s="140"/>
+      <c r="D4" s="140"/>
+      <c r="E4" s="140"/>
+      <c r="F4" s="140"/>
+      <c r="G4" s="140"/>
+      <c r="H4" s="140"/>
+      <c r="I4" s="140"/>
+      <c r="J4" s="140"/>
+      <c r="K4" s="140"/>
+      <c r="L4" s="140"/>
+      <c r="M4" s="140"/>
+      <c r="N4" s="140"/>
       <c r="O4" s="2" t="s">
         <v>47</v>
       </c>
@@ -32676,11 +32676,11 @@
       <c r="R4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="S4" s="136"/>
-      <c r="T4" s="136"/>
-      <c r="U4" s="136"/>
-      <c r="V4" s="136"/>
-      <c r="W4" s="153"/>
+      <c r="S4" s="140"/>
+      <c r="T4" s="140"/>
+      <c r="U4" s="140"/>
+      <c r="V4" s="140"/>
+      <c r="W4" s="150"/>
     </row>
     <row r="5" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C5" s="6">
@@ -33399,11 +33399,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="U3:U4"/>
-    <mergeCell ref="V3:V4"/>
     <mergeCell ref="W3:W4"/>
     <mergeCell ref="C2:W2"/>
     <mergeCell ref="L3:L4"/>
@@ -33418,6 +33413,11 @@
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="U3:U4"/>
+    <mergeCell ref="V3:V4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -33443,24 +33443,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C2" s="149" t="s">
+      <c r="C2" s="148" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="149"/>
-      <c r="E2" s="149"/>
-      <c r="F2" s="152"/>
-      <c r="G2" s="149" t="s">
+      <c r="D2" s="148"/>
+      <c r="E2" s="148"/>
+      <c r="F2" s="149"/>
+      <c r="G2" s="148" t="s">
         <v>60</v>
       </c>
-      <c r="H2" s="149"/>
-      <c r="I2" s="149"/>
+      <c r="H2" s="148"/>
+      <c r="I2" s="148"/>
       <c r="J2" s="8"/>
-      <c r="K2" s="152" t="s">
+      <c r="K2" s="149" t="s">
         <v>59</v>
       </c>
-      <c r="L2" s="154"/>
-      <c r="M2" s="154"/>
-      <c r="N2" s="155"/>
+      <c r="L2" s="151"/>
+      <c r="M2" s="151"/>
+      <c r="N2" s="152"/>
     </row>
     <row r="3" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C3" s="3" t="s">
@@ -34080,33 +34080,33 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A2" s="136" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="136" t="s">
+      <c r="A2" s="140" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="140" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="136"/>
-      <c r="D2" s="136"/>
-      <c r="E2" s="136"/>
-      <c r="F2" s="136"/>
-      <c r="G2" s="136"/>
-      <c r="H2" s="136"/>
-      <c r="I2" s="136"/>
-      <c r="J2" s="136"/>
-      <c r="K2" s="136"/>
-      <c r="L2" s="136"/>
-      <c r="M2" s="136"/>
-      <c r="N2" s="136"/>
-      <c r="O2" s="136"/>
-      <c r="P2" s="136"/>
-      <c r="Q2" s="136"/>
-      <c r="S2" s="175" t="s">
+      <c r="C2" s="140"/>
+      <c r="D2" s="140"/>
+      <c r="E2" s="140"/>
+      <c r="F2" s="140"/>
+      <c r="G2" s="140"/>
+      <c r="H2" s="140"/>
+      <c r="I2" s="140"/>
+      <c r="J2" s="140"/>
+      <c r="K2" s="140"/>
+      <c r="L2" s="140"/>
+      <c r="M2" s="140"/>
+      <c r="N2" s="140"/>
+      <c r="O2" s="140"/>
+      <c r="P2" s="140"/>
+      <c r="Q2" s="140"/>
+      <c r="S2" s="177" t="s">
         <v>69</v>
       </c>
-      <c r="T2" s="176"/>
-      <c r="U2" s="176"/>
-      <c r="V2" s="177"/>
+      <c r="T2" s="178"/>
+      <c r="U2" s="178"/>
+      <c r="V2" s="179"/>
       <c r="X2" t="s">
         <v>107</v>
       </c>
@@ -34169,7 +34169,7 @@
       </c>
     </row>
     <row r="3" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A3" s="136"/>
+      <c r="A3" s="140"/>
       <c r="B3" s="2" t="s">
         <v>65</v>
       </c>
@@ -34292,31 +34292,31 @@
       </c>
     </row>
     <row r="4" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A4" s="136"/>
-      <c r="B4" s="136" t="s">
+      <c r="A4" s="140"/>
+      <c r="B4" s="140" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="136"/>
-      <c r="D4" s="136"/>
-      <c r="E4" s="136"/>
-      <c r="F4" s="136"/>
-      <c r="G4" s="136"/>
-      <c r="H4" s="136"/>
-      <c r="I4" s="136"/>
-      <c r="J4" s="136"/>
-      <c r="K4" s="136"/>
-      <c r="L4" s="136"/>
-      <c r="M4" s="136"/>
-      <c r="N4" s="136"/>
-      <c r="O4" s="136"/>
-      <c r="P4" s="136"/>
-      <c r="Q4" s="136"/>
-      <c r="S4" s="136" t="s">
+      <c r="C4" s="140"/>
+      <c r="D4" s="140"/>
+      <c r="E4" s="140"/>
+      <c r="F4" s="140"/>
+      <c r="G4" s="140"/>
+      <c r="H4" s="140"/>
+      <c r="I4" s="140"/>
+      <c r="J4" s="140"/>
+      <c r="K4" s="140"/>
+      <c r="L4" s="140"/>
+      <c r="M4" s="140"/>
+      <c r="N4" s="140"/>
+      <c r="O4" s="140"/>
+      <c r="P4" s="140"/>
+      <c r="Q4" s="140"/>
+      <c r="S4" s="140" t="s">
         <v>75</v>
       </c>
-      <c r="T4" s="136"/>
-      <c r="U4" s="136"/>
-      <c r="V4" s="136"/>
+      <c r="T4" s="140"/>
+      <c r="U4" s="140"/>
+      <c r="V4" s="140"/>
       <c r="X4" t="s">
         <v>109</v>
       </c>
@@ -35769,82 +35769,82 @@
       <c r="Q24" s="14"/>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A25" s="136" t="s">
-        <v>0</v>
-      </c>
-      <c r="B25" s="136" t="s">
+      <c r="A25" s="140" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="140" t="s">
         <v>81</v>
       </c>
-      <c r="C25" s="136"/>
-      <c r="D25" s="136"/>
-      <c r="E25" s="136"/>
-      <c r="F25" s="136"/>
-      <c r="G25" s="136"/>
-      <c r="H25" s="136"/>
-      <c r="I25" s="136"/>
-      <c r="J25" s="136"/>
-      <c r="K25" s="136"/>
-      <c r="L25" s="136"/>
-      <c r="M25" s="136"/>
-      <c r="N25" s="136"/>
+      <c r="C25" s="140"/>
+      <c r="D25" s="140"/>
+      <c r="E25" s="140"/>
+      <c r="F25" s="140"/>
+      <c r="G25" s="140"/>
+      <c r="H25" s="140"/>
+      <c r="I25" s="140"/>
+      <c r="J25" s="140"/>
+      <c r="K25" s="140"/>
+      <c r="L25" s="140"/>
+      <c r="M25" s="140"/>
+      <c r="N25" s="140"/>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A26" s="136"/>
-      <c r="B26" s="136" t="s">
+      <c r="A26" s="140"/>
+      <c r="B26" s="140" t="s">
         <v>64</v>
       </c>
-      <c r="C26" s="136" t="s">
+      <c r="C26" s="140" t="s">
         <v>63</v>
       </c>
-      <c r="D26" s="136" t="s">
+      <c r="D26" s="140" t="s">
         <v>66</v>
       </c>
-      <c r="E26" s="136" t="s">
+      <c r="E26" s="140" t="s">
         <v>78</v>
       </c>
-      <c r="F26" s="136" t="s">
+      <c r="F26" s="140" t="s">
         <v>61</v>
       </c>
-      <c r="G26" s="136"/>
-      <c r="H26" s="136"/>
-      <c r="I26" s="136"/>
-      <c r="J26" s="136" t="s">
+      <c r="G26" s="140"/>
+      <c r="H26" s="140"/>
+      <c r="I26" s="140"/>
+      <c r="J26" s="140" t="s">
         <v>79</v>
       </c>
-      <c r="K26" s="136" t="s">
+      <c r="K26" s="140" t="s">
         <v>62</v>
       </c>
-      <c r="L26" s="136" t="s">
+      <c r="L26" s="140" t="s">
         <v>80</v>
       </c>
-      <c r="M26" s="136" t="s">
+      <c r="M26" s="140" t="s">
         <v>77</v>
       </c>
-      <c r="N26" s="136" t="s">
+      <c r="N26" s="140" t="s">
         <v>68</v>
       </c>
-      <c r="P26" s="136" t="s">
+      <c r="P26" s="140" t="s">
         <v>82</v>
       </c>
-      <c r="Q26" s="136" t="s">
+      <c r="Q26" s="140" t="s">
         <v>4</v>
       </c>
-      <c r="R26" s="136" t="s">
+      <c r="R26" s="140" t="s">
         <v>21</v>
       </c>
-      <c r="S26" s="136" t="s">
+      <c r="S26" s="140" t="s">
         <v>83</v>
       </c>
-      <c r="T26" s="153" t="s">
+      <c r="T26" s="150" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A27" s="136"/>
-      <c r="B27" s="136"/>
-      <c r="C27" s="136"/>
-      <c r="D27" s="136"/>
-      <c r="E27" s="136"/>
+      <c r="A27" s="140"/>
+      <c r="B27" s="140"/>
+      <c r="C27" s="140"/>
+      <c r="D27" s="140"/>
+      <c r="E27" s="140"/>
       <c r="F27" s="2" t="s">
         <v>2</v>
       </c>
@@ -35857,42 +35857,42 @@
       <c r="I27" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J27" s="136"/>
-      <c r="K27" s="136"/>
-      <c r="L27" s="136"/>
-      <c r="M27" s="136"/>
-      <c r="N27" s="136"/>
-      <c r="P27" s="136"/>
-      <c r="Q27" s="136"/>
-      <c r="R27" s="136"/>
-      <c r="S27" s="136"/>
-      <c r="T27" s="153"/>
+      <c r="J27" s="140"/>
+      <c r="K27" s="140"/>
+      <c r="L27" s="140"/>
+      <c r="M27" s="140"/>
+      <c r="N27" s="140"/>
+      <c r="P27" s="140"/>
+      <c r="Q27" s="140"/>
+      <c r="R27" s="140"/>
+      <c r="S27" s="140"/>
+      <c r="T27" s="150"/>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A28" s="136"/>
-      <c r="B28" s="136" t="s">
+      <c r="A28" s="140"/>
+      <c r="B28" s="140" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="136"/>
-      <c r="D28" s="136"/>
-      <c r="E28" s="136"/>
-      <c r="F28" s="136"/>
-      <c r="G28" s="136"/>
-      <c r="H28" s="136"/>
-      <c r="I28" s="136"/>
-      <c r="J28" s="136"/>
-      <c r="K28" s="136"/>
-      <c r="L28" s="136"/>
-      <c r="M28" s="136"/>
-      <c r="N28" s="136"/>
+      <c r="C28" s="140"/>
+      <c r="D28" s="140"/>
+      <c r="E28" s="140"/>
+      <c r="F28" s="140"/>
+      <c r="G28" s="140"/>
+      <c r="H28" s="140"/>
+      <c r="I28" s="140"/>
+      <c r="J28" s="140"/>
+      <c r="K28" s="140"/>
+      <c r="L28" s="140"/>
+      <c r="M28" s="140"/>
+      <c r="N28" s="140"/>
       <c r="O28" s="10"/>
-      <c r="P28" s="136" t="s">
+      <c r="P28" s="140" t="s">
         <v>26</v>
       </c>
-      <c r="Q28" s="136"/>
-      <c r="R28" s="136"/>
-      <c r="S28" s="136"/>
-      <c r="T28" s="136"/>
+      <c r="Q28" s="140"/>
+      <c r="R28" s="140"/>
+      <c r="S28" s="140"/>
+      <c r="T28" s="140"/>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
@@ -37130,47 +37130,47 @@
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="178" t="s">
-        <v>0</v>
-      </c>
-      <c r="B50" s="136" t="s">
+      <c r="A50" s="183" t="s">
+        <v>0</v>
+      </c>
+      <c r="B50" s="140" t="s">
         <v>85</v>
       </c>
-      <c r="C50" s="136"/>
-      <c r="D50" s="136" t="s">
+      <c r="C50" s="140"/>
+      <c r="D50" s="140" t="s">
         <v>87</v>
       </c>
-      <c r="E50" s="136"/>
-      <c r="F50" s="136"/>
-      <c r="G50" s="136"/>
-      <c r="H50" s="136"/>
-      <c r="I50" s="136"/>
+      <c r="E50" s="140"/>
+      <c r="F50" s="140"/>
+      <c r="G50" s="140"/>
+      <c r="H50" s="140"/>
+      <c r="I50" s="140"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="178"/>
-      <c r="B51" s="136" t="s">
+      <c r="A51" s="183"/>
+      <c r="B51" s="140" t="s">
         <v>26</v>
       </c>
-      <c r="C51" s="136" t="s">
+      <c r="C51" s="140" t="s">
         <v>86</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>88</v>
       </c>
       <c r="E51" s="2"/>
-      <c r="F51" s="136" t="s">
+      <c r="F51" s="140" t="s">
         <v>89</v>
       </c>
-      <c r="G51" s="136"/>
-      <c r="H51" s="136" t="s">
+      <c r="G51" s="140"/>
+      <c r="H51" s="140" t="s">
         <v>20</v>
       </c>
-      <c r="I51" s="136"/>
+      <c r="I51" s="140"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="179"/>
-      <c r="B52" s="136"/>
-      <c r="C52" s="136"/>
+      <c r="A52" s="184"/>
+      <c r="B52" s="140"/>
+      <c r="C52" s="140"/>
       <c r="D52" s="2" t="s">
         <v>26</v>
       </c>
@@ -37550,7 +37550,7 @@
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A74" s="149" t="s">
+      <c r="A74" s="148" t="s">
         <v>0</v>
       </c>
       <c r="B74" s="3" t="s">
@@ -37585,7 +37585,7 @@
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A75" s="149"/>
+      <c r="A75" s="148"/>
       <c r="B75" s="3" t="s">
         <v>115</v>
       </c>
@@ -37601,13 +37601,13 @@
       <c r="F75" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H75" s="152" t="s">
+      <c r="H75" s="149" t="s">
         <v>95</v>
       </c>
-      <c r="I75" s="154"/>
-      <c r="J75" s="154"/>
-      <c r="K75" s="154"/>
-      <c r="L75" s="155"/>
+      <c r="I75" s="151"/>
+      <c r="J75" s="151"/>
+      <c r="K75" s="151"/>
+      <c r="L75" s="152"/>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
@@ -38645,15 +38645,14 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="A74:A75"/>
-    <mergeCell ref="H75:L75"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="H51:I51"/>
-    <mergeCell ref="D50:I50"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="N26:N27"/>
+    <mergeCell ref="S4:V4"/>
+    <mergeCell ref="S2:V2"/>
+    <mergeCell ref="P26:P27"/>
+    <mergeCell ref="Q26:Q27"/>
+    <mergeCell ref="R26:R27"/>
+    <mergeCell ref="S26:S27"/>
+    <mergeCell ref="T26:T27"/>
     <mergeCell ref="A25:A28"/>
     <mergeCell ref="B28:N28"/>
     <mergeCell ref="A2:A4"/>
@@ -38670,14 +38669,15 @@
     <mergeCell ref="K26:K27"/>
     <mergeCell ref="L26:L27"/>
     <mergeCell ref="M26:M27"/>
-    <mergeCell ref="N26:N27"/>
-    <mergeCell ref="S4:V4"/>
-    <mergeCell ref="S2:V2"/>
-    <mergeCell ref="P26:P27"/>
-    <mergeCell ref="Q26:Q27"/>
-    <mergeCell ref="R26:R27"/>
-    <mergeCell ref="S26:S27"/>
-    <mergeCell ref="T26:T27"/>
+    <mergeCell ref="A74:A75"/>
+    <mergeCell ref="H75:L75"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="H51:I51"/>
+    <mergeCell ref="D50:I50"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="A50:A52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -38701,7 +38701,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B1" s="136" t="s">
+      <c r="B1" s="140" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -38751,26 +38751,26 @@
       </c>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="136"/>
-      <c r="C2" s="136" t="s">
+      <c r="B2" s="140"/>
+      <c r="C2" s="140" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="136"/>
-      <c r="E2" s="136"/>
-      <c r="F2" s="136"/>
-      <c r="G2" s="136"/>
-      <c r="H2" s="136"/>
-      <c r="I2" s="136"/>
-      <c r="J2" s="136"/>
-      <c r="K2" s="136"/>
-      <c r="M2" s="149" t="s">
+      <c r="D2" s="140"/>
+      <c r="E2" s="140"/>
+      <c r="F2" s="140"/>
+      <c r="G2" s="140"/>
+      <c r="H2" s="140"/>
+      <c r="I2" s="140"/>
+      <c r="J2" s="140"/>
+      <c r="K2" s="140"/>
+      <c r="M2" s="148" t="s">
         <v>95</v>
       </c>
-      <c r="N2" s="149"/>
-      <c r="O2" s="149"/>
-      <c r="P2" s="149"/>
-      <c r="Q2" s="149"/>
-      <c r="R2" s="149"/>
+      <c r="N2" s="148"/>
+      <c r="O2" s="148"/>
+      <c r="P2" s="148"/>
+      <c r="Q2" s="148"/>
+      <c r="R2" s="148"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" s="17">
@@ -39766,93 +39766,93 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A1" s="156" t="s">
+      <c r="A1" s="153" t="s">
         <v>224</v>
       </c>
-      <c r="B1" s="157"/>
-      <c r="C1" s="157"/>
-      <c r="D1" s="157"/>
-      <c r="E1" s="157"/>
-      <c r="F1" s="157"/>
-      <c r="G1" s="158"/>
-      <c r="H1" s="139" t="s">
+      <c r="B1" s="154"/>
+      <c r="C1" s="154"/>
+      <c r="D1" s="154"/>
+      <c r="E1" s="154"/>
+      <c r="F1" s="154"/>
+      <c r="G1" s="155"/>
+      <c r="H1" s="143" t="s">
         <v>225</v>
       </c>
-      <c r="I1" s="139"/>
-      <c r="J1" s="139"/>
-      <c r="K1" s="139"/>
-      <c r="L1" s="139"/>
-      <c r="M1" s="139"/>
-      <c r="N1" s="139"/>
+      <c r="I1" s="143"/>
+      <c r="J1" s="143"/>
+      <c r="K1" s="143"/>
+      <c r="L1" s="143"/>
+      <c r="M1" s="143"/>
+      <c r="N1" s="143"/>
       <c r="O1" s="132"/>
-      <c r="R1" s="149" t="s">
+      <c r="R1" s="148" t="s">
         <v>239</v>
       </c>
-      <c r="S1" s="149"/>
-      <c r="T1" s="149"/>
-      <c r="U1" s="149"/>
-      <c r="V1" s="149"/>
-      <c r="W1" s="149"/>
-      <c r="X1" s="149"/>
+      <c r="S1" s="148"/>
+      <c r="T1" s="148"/>
+      <c r="U1" s="148"/>
+      <c r="V1" s="148"/>
+      <c r="W1" s="148"/>
+      <c r="X1" s="148"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="160" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="159" t="s">
+      <c r="A2" s="157" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="156" t="s">
         <v>197</v>
       </c>
-      <c r="C2" s="159"/>
-      <c r="D2" s="159"/>
-      <c r="E2" s="160" t="s">
+      <c r="C2" s="156"/>
+      <c r="D2" s="156"/>
+      <c r="E2" s="157" t="s">
         <v>182</v>
       </c>
-      <c r="F2" s="160" t="s">
+      <c r="F2" s="157" t="s">
         <v>183</v>
       </c>
-      <c r="G2" s="147" t="s">
+      <c r="G2" s="158" t="s">
         <v>227</v>
       </c>
-      <c r="H2" s="143" t="s">
-        <v>0</v>
-      </c>
-      <c r="I2" s="139" t="s">
+      <c r="H2" s="161" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="143" t="s">
         <v>197</v>
       </c>
-      <c r="J2" s="139"/>
-      <c r="K2" s="139"/>
-      <c r="L2" s="143" t="s">
+      <c r="J2" s="143"/>
+      <c r="K2" s="143"/>
+      <c r="L2" s="161" t="s">
         <v>182</v>
       </c>
-      <c r="M2" s="143" t="s">
+      <c r="M2" s="161" t="s">
         <v>183</v>
       </c>
-      <c r="N2" s="144" t="s">
+      <c r="N2" s="162" t="s">
         <v>228</v>
       </c>
       <c r="O2" s="133" t="s">
         <v>420</v>
       </c>
-      <c r="R2" s="136" t="s">
-        <v>0</v>
-      </c>
-      <c r="S2" s="149" t="s">
+      <c r="R2" s="140" t="s">
+        <v>0</v>
+      </c>
+      <c r="S2" s="148" t="s">
         <v>197</v>
       </c>
-      <c r="T2" s="149"/>
-      <c r="U2" s="149"/>
-      <c r="V2" s="136" t="s">
+      <c r="T2" s="148"/>
+      <c r="U2" s="148"/>
+      <c r="V2" s="140" t="s">
         <v>182</v>
       </c>
-      <c r="W2" s="136" t="s">
+      <c r="W2" s="140" t="s">
         <v>183</v>
       </c>
-      <c r="X2" s="150" t="s">
+      <c r="X2" s="146" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" s="160"/>
+      <c r="A3" s="157"/>
       <c r="B3" s="128" t="s">
         <v>222</v>
       </c>
@@ -39862,10 +39862,10 @@
       <c r="D3" s="128" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="160"/>
-      <c r="F3" s="160"/>
-      <c r="G3" s="148"/>
-      <c r="H3" s="143"/>
+      <c r="E3" s="157"/>
+      <c r="F3" s="157"/>
+      <c r="G3" s="159"/>
+      <c r="H3" s="161"/>
       <c r="I3" s="25" t="s">
         <v>222</v>
       </c>
@@ -39875,9 +39875,9 @@
       <c r="K3" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="143"/>
-      <c r="M3" s="143"/>
-      <c r="N3" s="144"/>
+      <c r="L3" s="161"/>
+      <c r="M3" s="161"/>
+      <c r="N3" s="162"/>
       <c r="O3" s="133"/>
       <c r="P3" s="32">
         <v>8.5245999999999995</v>
@@ -39885,7 +39885,7 @@
       <c r="Q3" t="s">
         <v>226</v>
       </c>
-      <c r="R3" s="136"/>
+      <c r="R3" s="140"/>
       <c r="S3" s="3" t="s">
         <v>222</v>
       </c>
@@ -39895,9 +39895,9 @@
       <c r="U3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V3" s="136"/>
-      <c r="W3" s="136"/>
-      <c r="X3" s="151"/>
+      <c r="V3" s="140"/>
+      <c r="W3" s="140"/>
+      <c r="X3" s="147"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="83">
@@ -41488,7 +41488,7 @@
       <c r="F23" s="84">
         <v>5714693</v>
       </c>
-      <c r="G23" s="181"/>
+      <c r="G23" s="135"/>
       <c r="H23" s="44"/>
       <c r="R23" s="64">
         <v>2019</v>
@@ -41519,7 +41519,7 @@
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="G24" s="180">
+      <c r="G24" s="134">
         <f>E28*P5</f>
         <v>429447452.20999998</v>
       </c>
@@ -41548,38 +41548,38 @@
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A25" s="136" t="s">
-        <v>0</v>
-      </c>
-      <c r="B25" s="153" t="s">
+      <c r="A25" s="140" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="150" t="s">
         <v>249</v>
       </c>
-      <c r="C25" s="153" t="s">
+      <c r="C25" s="150" t="s">
         <v>250</v>
       </c>
-      <c r="D25" s="153" t="s">
+      <c r="D25" s="150" t="s">
         <v>251</v>
       </c>
-      <c r="E25" s="153" t="s">
+      <c r="E25" s="150" t="s">
         <v>261</v>
       </c>
-      <c r="F25" s="153" t="s">
+      <c r="F25" s="150" t="s">
         <v>85</v>
       </c>
-      <c r="G25" s="152" t="s">
+      <c r="G25" s="149" t="s">
         <v>257</v>
       </c>
-      <c r="H25" s="154"/>
-      <c r="I25" s="154"/>
-      <c r="J25" s="154"/>
-      <c r="K25" s="154"/>
-      <c r="L25" s="154"/>
-      <c r="M25" s="154"/>
-      <c r="N25" s="154"/>
-      <c r="O25" s="154"/>
-      <c r="P25" s="154"/>
-      <c r="Q25" s="154"/>
-      <c r="R25" s="155"/>
+      <c r="H25" s="151"/>
+      <c r="I25" s="151"/>
+      <c r="J25" s="151"/>
+      <c r="K25" s="151"/>
+      <c r="L25" s="151"/>
+      <c r="M25" s="151"/>
+      <c r="N25" s="151"/>
+      <c r="O25" s="151"/>
+      <c r="P25" s="151"/>
+      <c r="Q25" s="151"/>
+      <c r="R25" s="152"/>
       <c r="W25" t="s">
         <v>258</v>
       </c>
@@ -41591,12 +41591,12 @@
       </c>
     </row>
     <row r="26" spans="1:25" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="136"/>
-      <c r="B26" s="153"/>
-      <c r="C26" s="153"/>
-      <c r="D26" s="153"/>
-      <c r="E26" s="153"/>
-      <c r="F26" s="153"/>
+      <c r="A26" s="140"/>
+      <c r="B26" s="150"/>
+      <c r="C26" s="150"/>
+      <c r="D26" s="150"/>
+      <c r="E26" s="150"/>
+      <c r="F26" s="150"/>
       <c r="G26" s="3" t="s">
         <v>252</v>
       </c>
@@ -41618,40 +41618,40 @@
       <c r="M26" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N26" s="145" t="s">
+      <c r="N26" s="163" t="s">
         <v>391</v>
       </c>
-      <c r="O26" s="146"/>
-      <c r="P26" s="149" t="s">
+      <c r="O26" s="164"/>
+      <c r="P26" s="148" t="s">
         <v>392</v>
       </c>
-      <c r="Q26" s="149"/>
-      <c r="R26" s="152"/>
+      <c r="Q26" s="148"/>
+      <c r="R26" s="149"/>
       <c r="S26" s="127" t="s">
         <v>393</v>
       </c>
-      <c r="T26" s="142" t="s">
+      <c r="T26" s="160" t="s">
         <v>394</v>
       </c>
-      <c r="U26" s="142"/>
+      <c r="U26" s="160"/>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A27" s="136"/>
-      <c r="B27" s="149" t="s">
+      <c r="A27" s="140"/>
+      <c r="B27" s="148" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="149"/>
-      <c r="D27" s="149"/>
-      <c r="E27" s="149"/>
-      <c r="F27" s="149"/>
-      <c r="G27" s="149"/>
-      <c r="H27" s="149"/>
-      <c r="I27" s="149"/>
-      <c r="J27" s="149"/>
-      <c r="K27" s="149"/>
-      <c r="L27" s="149"/>
-      <c r="M27" s="149"/>
-      <c r="N27" s="149"/>
+      <c r="C27" s="148"/>
+      <c r="D27" s="148"/>
+      <c r="E27" s="148"/>
+      <c r="F27" s="148"/>
+      <c r="G27" s="148"/>
+      <c r="H27" s="148"/>
+      <c r="I27" s="148"/>
+      <c r="J27" s="148"/>
+      <c r="K27" s="148"/>
+      <c r="L27" s="148"/>
+      <c r="M27" s="148"/>
+      <c r="N27" s="148"/>
       <c r="O27" s="123" t="s">
         <v>95</v>
       </c>
@@ -43213,47 +43213,47 @@
       </c>
     </row>
     <row r="48" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A48" s="183">
+      <c r="A48" s="137">
         <v>2020</v>
       </c>
-      <c r="B48" s="183">
+      <c r="B48" s="137">
         <v>2442831</v>
       </c>
-      <c r="C48" s="183">
+      <c r="C48" s="137">
         <v>139469</v>
       </c>
-      <c r="D48" s="183">
+      <c r="D48" s="137">
         <v>213399</v>
       </c>
-      <c r="E48" s="183">
+      <c r="E48" s="137">
         <f t="shared" si="29"/>
         <v>2089963</v>
       </c>
-      <c r="F48" s="183">
+      <c r="F48" s="137">
         <v>174223</v>
       </c>
-      <c r="G48" s="183">
+      <c r="G48" s="137">
         <v>818900</v>
       </c>
-      <c r="H48" s="183">
+      <c r="H48" s="137">
         <v>18468</v>
       </c>
-      <c r="I48" s="183">
+      <c r="I48" s="137">
         <v>13897</v>
       </c>
-      <c r="J48" s="183">
+      <c r="J48" s="137">
         <v>8046</v>
       </c>
-      <c r="K48" s="183">
+      <c r="K48" s="137">
         <v>139592</v>
       </c>
-      <c r="L48" s="183">
+      <c r="L48" s="137">
         <v>673806</v>
       </c>
-      <c r="M48" s="183">
+      <c r="M48" s="137">
         <v>249876</v>
       </c>
-      <c r="N48" s="183">
+      <c r="N48" s="137">
         <v>184180</v>
       </c>
       <c r="O48" s="3">
@@ -43268,12 +43268,12 @@
       <c r="C49" t="s">
         <v>182</v>
       </c>
-      <c r="K49" s="184" t="s">
+      <c r="K49" s="165" t="s">
         <v>112</v>
       </c>
-      <c r="L49" s="184"/>
-      <c r="M49" s="184"/>
-      <c r="N49" s="184"/>
+      <c r="L49" s="165"/>
+      <c r="M49" s="165"/>
+      <c r="N49" s="165"/>
     </row>
     <row r="50" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B50">
@@ -43327,21 +43327,21 @@
       <c r="G51" s="28" t="s">
         <v>404</v>
       </c>
-      <c r="H51" s="139" t="s">
+      <c r="H51" s="143" t="s">
         <v>95</v>
       </c>
-      <c r="I51" s="134"/>
+      <c r="I51" s="138"/>
       <c r="J51" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="K51" s="139" t="s">
+      <c r="K51" s="143" t="s">
         <v>95</v>
       </c>
-      <c r="L51" s="139"/>
-      <c r="M51" s="139"/>
-      <c r="N51" s="139"/>
-      <c r="O51" s="139"/>
-      <c r="P51" s="139"/>
+      <c r="L51" s="143"/>
+      <c r="M51" s="143"/>
+      <c r="N51" s="143"/>
+      <c r="O51" s="143"/>
+      <c r="P51" s="143"/>
     </row>
     <row r="52" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B52">
@@ -44597,6 +44597,22 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="H51:I51"/>
+    <mergeCell ref="T26:U26"/>
+    <mergeCell ref="W2:W3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="K49:N49"/>
+    <mergeCell ref="K51:P51"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H1:N1"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="S2:U2"/>
+    <mergeCell ref="V2:V3"/>
     <mergeCell ref="A25:A27"/>
     <mergeCell ref="X2:X3"/>
     <mergeCell ref="R1:X1"/>
@@ -44613,22 +44629,6 @@
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="H1:N1"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="S2:U2"/>
-    <mergeCell ref="V2:V3"/>
-    <mergeCell ref="H51:I51"/>
-    <mergeCell ref="T26:U26"/>
-    <mergeCell ref="W2:W3"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="N26:O26"/>
-    <mergeCell ref="K49:N49"/>
-    <mergeCell ref="K51:P51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -44830,38 +44830,38 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B1" s="141" t="s">
+      <c r="B1" s="145" t="s">
         <v>357</v>
       </c>
-      <c r="C1" s="141"/>
-      <c r="D1" s="141" t="s">
+      <c r="C1" s="145"/>
+      <c r="D1" s="145" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="141"/>
-      <c r="F1" s="141" t="s">
+      <c r="E1" s="145"/>
+      <c r="F1" s="145" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="141"/>
-      <c r="H1" s="141" t="s">
+      <c r="G1" s="145"/>
+      <c r="H1" s="145" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="141"/>
-      <c r="J1" s="141" t="s">
+      <c r="I1" s="145"/>
+      <c r="J1" s="145" t="s">
         <v>99</v>
       </c>
-      <c r="K1" s="141"/>
-      <c r="L1" s="141" t="s">
+      <c r="K1" s="145"/>
+      <c r="L1" s="145" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="141"/>
-      <c r="N1" s="141" t="s">
+      <c r="M1" s="145"/>
+      <c r="N1" s="145" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="141"/>
-      <c r="P1" s="141" t="s">
+      <c r="O1" s="145"/>
+      <c r="P1" s="145" t="s">
         <v>356</v>
       </c>
-      <c r="Q1" s="141"/>
+      <c r="Q1" s="145"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -46550,13 +46550,13 @@
       <c r="B1" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="C1" s="149" t="s">
+      <c r="C1" s="148" t="s">
         <v>346</v>
       </c>
-      <c r="D1" s="149"/>
-      <c r="E1" s="149"/>
-      <c r="F1" s="149"/>
-      <c r="G1" s="149"/>
+      <c r="D1" s="148"/>
+      <c r="E1" s="148"/>
+      <c r="F1" s="148"/>
+      <c r="G1" s="148"/>
       <c r="L1">
         <v>0.17245495999999999</v>
       </c>
@@ -47502,13 +47502,13 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="107"/>
-      <c r="B1" s="161" t="s">
+      <c r="B1" s="166" t="s">
         <v>335</v>
       </c>
-      <c r="C1" s="161"/>
-      <c r="D1" s="161"/>
-      <c r="E1" s="161"/>
-      <c r="F1" s="161"/>
+      <c r="C1" s="166"/>
+      <c r="D1" s="166"/>
+      <c r="E1" s="166"/>
+      <c r="F1" s="166"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="108" t="s">
@@ -48115,22 +48115,22 @@
       </c>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C2" s="144" t="s">
+      <c r="C2" s="162" t="s">
         <v>95</v>
       </c>
-      <c r="D2" s="144"/>
-      <c r="E2" s="144"/>
-      <c r="F2" s="144"/>
-      <c r="G2" s="144"/>
-      <c r="H2" s="144"/>
-      <c r="I2" s="144"/>
-      <c r="J2" s="144"/>
-      <c r="K2" s="144"/>
-      <c r="L2" s="144"/>
-      <c r="M2" s="144"/>
-      <c r="N2" s="144"/>
-      <c r="O2" s="144"/>
-      <c r="P2" s="144"/>
+      <c r="D2" s="162"/>
+      <c r="E2" s="162"/>
+      <c r="F2" s="162"/>
+      <c r="G2" s="162"/>
+      <c r="H2" s="162"/>
+      <c r="I2" s="162"/>
+      <c r="J2" s="162"/>
+      <c r="K2" s="162"/>
+      <c r="L2" s="162"/>
+      <c r="M2" s="162"/>
+      <c r="N2" s="162"/>
+      <c r="O2" s="162"/>
+      <c r="P2" s="162"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" s="3">
@@ -49000,11 +49000,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B1" s="162" t="s">
+      <c r="B1" s="167" t="s">
         <v>184</v>
       </c>
-      <c r="C1" s="162"/>
-      <c r="D1" s="162"/>
+      <c r="C1" s="167"/>
+      <c r="D1" s="167"/>
       <c r="E1" s="46" t="s">
         <v>185</v>
       </c>
@@ -49014,20 +49014,20 @@
       <c r="G1" s="46" t="s">
         <v>186</v>
       </c>
-      <c r="H1" s="164" t="s">
+      <c r="H1" s="169" t="s">
         <v>187</v>
       </c>
-      <c r="I1" s="164"/>
-      <c r="J1" s="164"/>
-      <c r="K1" s="164"/>
-      <c r="L1" s="164"/>
-      <c r="M1" s="163" t="s">
+      <c r="I1" s="169"/>
+      <c r="J1" s="169"/>
+      <c r="K1" s="169"/>
+      <c r="L1" s="169"/>
+      <c r="M1" s="168" t="s">
         <v>188</v>
       </c>
-      <c r="N1" s="141"/>
-      <c r="O1" s="141"/>
-      <c r="P1" s="141"/>
-      <c r="Q1" s="141"/>
+      <c r="N1" s="145"/>
+      <c r="O1" s="145"/>
+      <c r="P1" s="145"/>
+      <c r="Q1" s="145"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B2" s="47" t="s">
@@ -49800,13 +49800,13 @@
       <c r="A23">
         <v>2020</v>
       </c>
-      <c r="B23" s="182">
+      <c r="B23" s="136">
         <v>563728255</v>
       </c>
-      <c r="C23" s="182">
+      <c r="C23" s="136">
         <v>405052868</v>
       </c>
-      <c r="D23" s="182">
+      <c r="D23" s="136">
         <v>8756363</v>
       </c>
       <c r="E23" s="49">
@@ -50899,64 +50899,64 @@
       </c>
     </row>
     <row r="50" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B50" s="149" t="s">
+      <c r="B50" s="148" t="s">
         <v>423</v>
       </c>
-      <c r="C50" s="149"/>
-      <c r="D50" s="149"/>
-      <c r="E50" s="149"/>
-      <c r="F50" s="149"/>
-      <c r="G50" s="149"/>
-      <c r="H50" s="149"/>
-      <c r="I50" s="149"/>
-      <c r="J50" s="149"/>
-      <c r="K50" s="149"/>
-      <c r="L50" s="149"/>
-      <c r="M50" s="149"/>
-      <c r="P50" s="149" t="s">
+      <c r="C50" s="148"/>
+      <c r="D50" s="148"/>
+      <c r="E50" s="148"/>
+      <c r="F50" s="148"/>
+      <c r="G50" s="148"/>
+      <c r="H50" s="148"/>
+      <c r="I50" s="148"/>
+      <c r="J50" s="148"/>
+      <c r="K50" s="148"/>
+      <c r="L50" s="148"/>
+      <c r="M50" s="148"/>
+      <c r="P50" s="148" t="s">
         <v>423</v>
       </c>
-      <c r="Q50" s="149"/>
-      <c r="R50" s="149"/>
-      <c r="S50" s="149"/>
-      <c r="T50" s="149"/>
-      <c r="U50" s="149"/>
-      <c r="V50" s="149"/>
-      <c r="W50" s="149"/>
-      <c r="X50" s="149"/>
-      <c r="Y50" s="149"/>
-      <c r="Z50" s="149"/>
-      <c r="AA50" s="149"/>
+      <c r="Q50" s="148"/>
+      <c r="R50" s="148"/>
+      <c r="S50" s="148"/>
+      <c r="T50" s="148"/>
+      <c r="U50" s="148"/>
+      <c r="V50" s="148"/>
+      <c r="W50" s="148"/>
+      <c r="X50" s="148"/>
+      <c r="Y50" s="148"/>
+      <c r="Z50" s="148"/>
+      <c r="AA50" s="148"/>
     </row>
     <row r="51" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B51" s="149" t="s">
+      <c r="B51" s="148" t="s">
         <v>438</v>
       </c>
-      <c r="C51" s="149"/>
-      <c r="D51" s="149"/>
-      <c r="E51" s="149"/>
-      <c r="F51" s="149"/>
-      <c r="G51" s="149"/>
-      <c r="H51" s="149"/>
-      <c r="I51" s="149"/>
-      <c r="J51" s="149"/>
-      <c r="K51" s="149"/>
-      <c r="L51" s="149"/>
-      <c r="M51" s="149"/>
-      <c r="P51" s="149" t="s">
+      <c r="C51" s="148"/>
+      <c r="D51" s="148"/>
+      <c r="E51" s="148"/>
+      <c r="F51" s="148"/>
+      <c r="G51" s="148"/>
+      <c r="H51" s="148"/>
+      <c r="I51" s="148"/>
+      <c r="J51" s="148"/>
+      <c r="K51" s="148"/>
+      <c r="L51" s="148"/>
+      <c r="M51" s="148"/>
+      <c r="P51" s="148" t="s">
         <v>115</v>
       </c>
-      <c r="Q51" s="149"/>
-      <c r="R51" s="149"/>
-      <c r="S51" s="149"/>
-      <c r="T51" s="149"/>
-      <c r="U51" s="149"/>
-      <c r="V51" s="149"/>
-      <c r="W51" s="149"/>
-      <c r="X51" s="149"/>
-      <c r="Y51" s="149"/>
-      <c r="Z51" s="149"/>
-      <c r="AA51" s="149"/>
+      <c r="Q51" s="148"/>
+      <c r="R51" s="148"/>
+      <c r="S51" s="148"/>
+      <c r="T51" s="148"/>
+      <c r="U51" s="148"/>
+      <c r="V51" s="148"/>
+      <c r="W51" s="148"/>
+      <c r="X51" s="148"/>
+      <c r="Y51" s="148"/>
+      <c r="Z51" s="148"/>
+      <c r="AA51" s="148"/>
     </row>
     <row r="52" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
@@ -52875,36 +52875,36 @@
       </c>
     </row>
     <row r="75" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B75" s="149" t="s">
+      <c r="B75" s="148" t="s">
         <v>423</v>
       </c>
-      <c r="C75" s="149"/>
-      <c r="D75" s="149"/>
-      <c r="E75" s="149"/>
-      <c r="F75" s="149"/>
-      <c r="G75" s="149"/>
-      <c r="H75" s="149"/>
-      <c r="I75" s="149"/>
-      <c r="J75" s="149"/>
-      <c r="K75" s="149"/>
-      <c r="L75" s="149"/>
-      <c r="M75" s="149"/>
+      <c r="C75" s="148"/>
+      <c r="D75" s="148"/>
+      <c r="E75" s="148"/>
+      <c r="F75" s="148"/>
+      <c r="G75" s="148"/>
+      <c r="H75" s="148"/>
+      <c r="I75" s="148"/>
+      <c r="J75" s="148"/>
+      <c r="K75" s="148"/>
+      <c r="L75" s="148"/>
+      <c r="M75" s="148"/>
     </row>
     <row r="76" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B76" s="149" t="s">
+      <c r="B76" s="148" t="s">
         <v>95</v>
       </c>
-      <c r="C76" s="149"/>
-      <c r="D76" s="149"/>
-      <c r="E76" s="149"/>
-      <c r="F76" s="149"/>
-      <c r="G76" s="149"/>
-      <c r="H76" s="149"/>
-      <c r="I76" s="149"/>
-      <c r="J76" s="149"/>
-      <c r="K76" s="149"/>
-      <c r="L76" s="149"/>
-      <c r="M76" s="149"/>
+      <c r="C76" s="148"/>
+      <c r="D76" s="148"/>
+      <c r="E76" s="148"/>
+      <c r="F76" s="148"/>
+      <c r="G76" s="148"/>
+      <c r="H76" s="148"/>
+      <c r="I76" s="148"/>
+      <c r="J76" s="148"/>
+      <c r="K76" s="148"/>
+      <c r="L76" s="148"/>
+      <c r="M76" s="148"/>
     </row>
     <row r="77" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
@@ -54081,7 +54081,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B158D003-6CE6-47DC-9594-4C83C40B7901}">
   <dimension ref="A1:T74"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="N54" sqref="N54:N74"/>
     </sheetView>
   </sheetViews>
@@ -54091,10 +54091,10 @@
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.28515625" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.140625" bestFit="1" customWidth="1"/>
@@ -54107,7 +54107,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="136" t="s">
+      <c r="A1" s="140" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -54123,7 +54123,7 @@
         <v>198</v>
       </c>
       <c r="F1" s="3"/>
-      <c r="G1" s="165" t="s">
+      <c r="G1" s="170" t="s">
         <v>0</v>
       </c>
       <c r="H1" s="3" t="s">
@@ -54145,32 +54145,32 @@
         <v>286</v>
       </c>
       <c r="N1" s="95"/>
-      <c r="O1" s="141" t="s">
+      <c r="O1" s="145" t="s">
         <v>282</v>
       </c>
-      <c r="P1" s="141"/>
-      <c r="Q1" s="141"/>
-      <c r="R1" s="141"/>
-      <c r="S1" s="141"/>
+      <c r="P1" s="145"/>
+      <c r="Q1" s="145"/>
+      <c r="R1" s="145"/>
+      <c r="S1" s="145"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="136"/>
-      <c r="B2" s="149" t="s">
+      <c r="A2" s="140"/>
+      <c r="B2" s="148" t="s">
         <v>199</v>
       </c>
-      <c r="C2" s="149"/>
-      <c r="D2" s="149"/>
-      <c r="E2" s="149"/>
+      <c r="C2" s="148"/>
+      <c r="D2" s="148"/>
+      <c r="E2" s="148"/>
       <c r="F2" s="54" t="s">
         <v>200</v>
       </c>
-      <c r="G2" s="165"/>
-      <c r="H2" s="149" t="s">
+      <c r="G2" s="170"/>
+      <c r="H2" s="148" t="s">
         <v>201</v>
       </c>
-      <c r="I2" s="149"/>
-      <c r="J2" s="149"/>
-      <c r="K2" s="149"/>
+      <c r="I2" s="148"/>
+      <c r="J2" s="148"/>
+      <c r="K2" s="148"/>
       <c r="L2" s="99"/>
       <c r="N2" t="s">
         <v>218</v>
@@ -55742,11 +55742,11 @@
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B24" s="141" t="s">
+      <c r="B24" s="145" t="s">
         <v>196</v>
       </c>
-      <c r="C24" s="141"/>
-      <c r="D24" s="141"/>
+      <c r="C24" s="145"/>
+      <c r="D24" s="145"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B25" s="53"/>
@@ -55984,22 +55984,22 @@
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B51" s="149" t="s">
+      <c r="B51" s="148" t="s">
         <v>437</v>
       </c>
-      <c r="C51" s="149"/>
-      <c r="D51" s="149"/>
-      <c r="E51" s="149"/>
-      <c r="F51" s="149"/>
-      <c r="G51" s="149"/>
-      <c r="H51" s="149"/>
-      <c r="I51" s="149"/>
-      <c r="J51" s="149"/>
-      <c r="K51" s="149"/>
-      <c r="L51" s="149"/>
-      <c r="M51" s="149"/>
-      <c r="N51" s="149"/>
-      <c r="O51" s="149"/>
+      <c r="C51" s="148"/>
+      <c r="D51" s="148"/>
+      <c r="E51" s="148"/>
+      <c r="F51" s="148"/>
+      <c r="G51" s="148"/>
+      <c r="H51" s="148"/>
+      <c r="I51" s="148"/>
+      <c r="J51" s="148"/>
+      <c r="K51" s="148"/>
+      <c r="L51" s="148"/>
+      <c r="M51" s="148"/>
+      <c r="N51" s="148"/>
+      <c r="O51" s="148"/>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B52" s="3" t="s">
@@ -56046,24 +56046,24 @@
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B53" s="149" t="s">
+      <c r="B53" s="148" t="s">
         <v>436</v>
       </c>
-      <c r="C53" s="149"/>
-      <c r="D53" s="149"/>
-      <c r="E53" s="149"/>
-      <c r="F53" s="149"/>
-      <c r="G53" s="149"/>
-      <c r="H53" s="149"/>
-      <c r="I53" s="149" t="s">
+      <c r="C53" s="148"/>
+      <c r="D53" s="148"/>
+      <c r="E53" s="148"/>
+      <c r="F53" s="148"/>
+      <c r="G53" s="148"/>
+      <c r="H53" s="148"/>
+      <c r="I53" s="148" t="s">
         <v>95</v>
       </c>
-      <c r="J53" s="149"/>
-      <c r="K53" s="149"/>
-      <c r="L53" s="149"/>
-      <c r="M53" s="149"/>
-      <c r="N53" s="149"/>
-      <c r="O53" s="149"/>
+      <c r="J53" s="148"/>
+      <c r="K53" s="148"/>
+      <c r="L53" s="148"/>
+      <c r="M53" s="148"/>
+      <c r="N53" s="148"/>
+      <c r="O53" s="148"/>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54">
@@ -57201,6 +57201,8 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="H2:K2"/>
     <mergeCell ref="B53:H53"/>
     <mergeCell ref="I53:O53"/>
     <mergeCell ref="B51:O51"/>
@@ -57208,8 +57210,6 @@
     <mergeCell ref="B24:D24"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="G1:G2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="H2:K2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -57533,11 +57533,11 @@
         <v>119125379</v>
       </c>
       <c r="R3">
-        <f t="shared" ref="R3:R22" si="6">C3</f>
+        <f t="shared" ref="R3:R20" si="6">C3</f>
         <v>441731352</v>
       </c>
       <c r="S3">
-        <f t="shared" ref="S3:S22" si="7">D3</f>
+        <f t="shared" ref="S3:S20" si="7">D3</f>
         <v>172083907</v>
       </c>
       <c r="T3">
@@ -59927,7 +59927,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:36" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:36" ht="30" x14ac:dyDescent="0.25">
       <c r="B24" s="62" t="s">
         <v>178</v>
       </c>
@@ -59943,10 +59943,10 @@
       <c r="G24" s="20" t="s">
         <v>231</v>
       </c>
-      <c r="H24" s="167">
+      <c r="H24" s="171">
         <v>2132298</v>
       </c>
-      <c r="I24" s="168" t="s">
+      <c r="I24" s="172" t="s">
         <v>209</v>
       </c>
       <c r="K24" s="2" t="s">
@@ -59990,8 +59990,8 @@
         <f>D2*$H$44</f>
         <v>955101.35158651904</v>
       </c>
-      <c r="H25" s="167"/>
-      <c r="I25" s="168"/>
+      <c r="H25" s="171"/>
+      <c r="I25" s="172"/>
       <c r="K25" s="3">
         <v>2000</v>
       </c>
@@ -60039,8 +60039,8 @@
         <f t="shared" ref="G26:G43" si="48">D3*$H$44</f>
         <v>998224.41556934861</v>
       </c>
-      <c r="H26" s="167"/>
-      <c r="I26" s="168"/>
+      <c r="H26" s="171"/>
+      <c r="I26" s="172"/>
       <c r="K26" s="3">
         <v>2001</v>
       </c>
@@ -60088,8 +60088,8 @@
         <f t="shared" si="48"/>
         <v>1095320.5754394107</v>
       </c>
-      <c r="H27" s="167"/>
-      <c r="I27" s="168"/>
+      <c r="H27" s="171"/>
+      <c r="I27" s="172"/>
       <c r="K27" s="3">
         <v>2002</v>
       </c>
@@ -60137,8 +60137,8 @@
         <f t="shared" si="48"/>
         <v>1184187.3310516851</v>
       </c>
-      <c r="H28" s="167"/>
-      <c r="I28" s="168"/>
+      <c r="H28" s="171"/>
+      <c r="I28" s="172"/>
       <c r="K28" s="3">
         <v>2003</v>
       </c>
@@ -60186,8 +60186,8 @@
         <f t="shared" si="48"/>
         <v>1087962.0395614596</v>
       </c>
-      <c r="H29" s="167"/>
-      <c r="I29" s="168"/>
+      <c r="H29" s="171"/>
+      <c r="I29" s="172"/>
       <c r="K29" s="3">
         <v>2004</v>
       </c>
@@ -60235,8 +60235,8 @@
         <f t="shared" si="48"/>
         <v>1109051.429897326</v>
       </c>
-      <c r="H30" s="167"/>
-      <c r="I30" s="168"/>
+      <c r="H30" s="171"/>
+      <c r="I30" s="172"/>
       <c r="K30" s="3">
         <v>2005</v>
       </c>
@@ -60284,8 +60284,8 @@
         <f t="shared" si="48"/>
         <v>1140433.8186669762</v>
       </c>
-      <c r="H31" s="167"/>
-      <c r="I31" s="168"/>
+      <c r="H31" s="171"/>
+      <c r="I31" s="172"/>
       <c r="K31" s="3">
         <v>2006</v>
       </c>
@@ -60333,8 +60333,8 @@
         <f t="shared" si="48"/>
         <v>1065164.0814432392</v>
       </c>
-      <c r="H32" s="167"/>
-      <c r="I32" s="168"/>
+      <c r="H32" s="171"/>
+      <c r="I32" s="172"/>
       <c r="K32" s="3">
         <v>2007</v>
       </c>
@@ -60387,8 +60387,8 @@
         <f t="shared" si="48"/>
         <v>1369276.4429491272</v>
       </c>
-      <c r="H33" s="167"/>
-      <c r="I33" s="168"/>
+      <c r="H33" s="171"/>
+      <c r="I33" s="172"/>
       <c r="K33" s="3">
         <v>2008</v>
       </c>
@@ -60441,8 +60441,8 @@
         <f t="shared" si="48"/>
         <v>1456205.4063460759</v>
       </c>
-      <c r="H34" s="167"/>
-      <c r="I34" s="168"/>
+      <c r="H34" s="171"/>
+      <c r="I34" s="172"/>
       <c r="K34" s="3">
         <v>2009</v>
       </c>
@@ -60495,8 +60495,8 @@
         <f t="shared" si="48"/>
         <v>1565880.7645455075</v>
       </c>
-      <c r="H35" s="167"/>
-      <c r="I35" s="168"/>
+      <c r="H35" s="171"/>
+      <c r="I35" s="172"/>
       <c r="K35" s="3">
         <v>2010</v>
       </c>
@@ -60549,8 +60549,8 @@
         <f t="shared" si="48"/>
         <v>1518117.8258599688</v>
       </c>
-      <c r="H36" s="167"/>
-      <c r="I36" s="168"/>
+      <c r="H36" s="171"/>
+      <c r="I36" s="172"/>
       <c r="K36" s="3">
         <v>2011</v>
       </c>
@@ -60603,8 +60603,8 @@
         <f t="shared" si="48"/>
         <v>1505054.8987760313</v>
       </c>
-      <c r="H37" s="167"/>
-      <c r="I37" s="168"/>
+      <c r="H37" s="171"/>
+      <c r="I37" s="172"/>
       <c r="K37" s="3">
         <v>2012</v>
       </c>
@@ -60657,8 +60657,8 @@
         <f t="shared" si="48"/>
         <v>1348105.7891989097</v>
       </c>
-      <c r="H38" s="167"/>
-      <c r="I38" s="168"/>
+      <c r="H38" s="171"/>
+      <c r="I38" s="172"/>
       <c r="K38" s="3">
         <v>2013</v>
       </c>
@@ -60715,8 +60715,8 @@
         <f t="shared" si="48"/>
         <v>1574194.3906259066</v>
       </c>
-      <c r="H39" s="167"/>
-      <c r="I39" s="168"/>
+      <c r="H39" s="171"/>
+      <c r="I39" s="172"/>
       <c r="K39" s="3">
         <v>2014</v>
       </c>
@@ -60774,8 +60774,8 @@
         <f t="shared" si="48"/>
         <v>1597921.2251290679</v>
       </c>
-      <c r="H40" s="167"/>
-      <c r="I40" s="168"/>
+      <c r="H40" s="171"/>
+      <c r="I40" s="172"/>
       <c r="K40" s="3">
         <v>2015</v>
       </c>
@@ -60829,8 +60829,8 @@
         <f t="shared" si="48"/>
         <v>1607806.4678925693</v>
       </c>
-      <c r="H41" s="167"/>
-      <c r="I41" s="168"/>
+      <c r="H41" s="171"/>
+      <c r="I41" s="172"/>
       <c r="K41" s="3">
         <v>2016</v>
       </c>
@@ -60884,8 +60884,8 @@
         <f t="shared" si="48"/>
         <v>1596045.1708335751</v>
       </c>
-      <c r="H42" s="167"/>
-      <c r="I42" s="168"/>
+      <c r="H42" s="171"/>
+      <c r="I42" s="172"/>
       <c r="K42" s="3">
         <v>2017</v>
       </c>
@@ -60939,8 +60939,8 @@
         <f t="shared" si="48"/>
         <v>1672433.5228261501</v>
       </c>
-      <c r="H43" s="167"/>
-      <c r="I43" s="168"/>
+      <c r="H43" s="171"/>
+      <c r="I43" s="172"/>
       <c r="K43" s="3">
         <v>2018</v>
       </c>
@@ -60995,11 +60995,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E70ADBEC-D4B6-43FE-BDD8-10D822D35B73}">
   <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A23" sqref="A23"/>
+      <selection pane="bottomRight" activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>